<commit_message>
Setup of Bitmap Ops
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\coding\dotPDFium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A7B29D1-E049-4CF1-BD14-9719A2B7AD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB94E5A-865D-49EB-92A3-ABE264830B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38800" yWindow="750" windowWidth="33090" windowHeight="15370" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
+    <workbookView xWindow="3890" yWindow="3480" windowWidth="33090" windowHeight="15370" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="201">
   <si>
     <t>Text_LoadPage</t>
   </si>
@@ -636,6 +636,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Text_GetRect</t>
   </si>
 </sst>
 </file>
@@ -1040,7 +1043,7 @@
   <dimension ref="A1:R66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1296,6 +1299,9 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="B8" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="C8" t="s">
         <v>23</v>
       </c>
@@ -1322,6 +1328,9 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="B9" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="C9" t="s">
         <v>24</v>
       </c>
@@ -1343,7 +1352,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>200</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
@@ -1366,7 +1375,10 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="C11" t="s">
         <v>26</v>
@@ -1389,7 +1401,10 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="C12" t="s">
         <v>27</v>
@@ -1412,7 +1427,10 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>
@@ -1429,7 +1447,10 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="C14" t="s">
         <v>29</v>
@@ -1443,7 +1464,10 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
@@ -1457,7 +1481,10 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="C16" t="s">
         <v>31</v>
@@ -1467,6 +1494,9 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
       <c r="C17" t="s">
         <v>32</v>
       </c>
@@ -1528,7 +1558,6 @@
       </c>
     </row>
     <row r="28" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="1"/>
       <c r="B28" s="3"/>
       <c r="C28" s="1"/>
       <c r="D28" s="3"/>

</xml_diff>

<commit_message>
Render to bitmap and device <-> page coordinates.
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\coding\dotPDFium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB94E5A-865D-49EB-92A3-ABE264830B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27A5535-F3BD-4560-9C2F-5AE5695165EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3890" yWindow="3480" windowWidth="33090" windowHeight="15370" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
+    <workbookView xWindow="39090" yWindow="580" windowWidth="29750" windowHeight="15370" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="202">
   <si>
     <t>Text_LoadPage</t>
   </si>
@@ -639,6 +639,9 @@
   </si>
   <si>
     <t>Text_GetRect</t>
+  </si>
+  <si>
+    <t>xx</t>
   </si>
 </sst>
 </file>
@@ -1043,7 +1046,7 @@
   <dimension ref="A1:R66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1354,6 +1357,9 @@
       <c r="A10" t="s">
         <v>200</v>
       </c>
+      <c r="B10" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="C10" t="s">
         <v>25</v>
       </c>
@@ -1455,6 +1461,9 @@
       <c r="C14" t="s">
         <v>29</v>
       </c>
+      <c r="D14" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="M14" t="s">
         <v>90</v>
       </c>
@@ -1472,6 +1481,9 @@
       <c r="C15" t="s">
         <v>30</v>
       </c>
+      <c r="D15" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="M15" t="s">
         <v>91</v>
       </c>
@@ -1489,6 +1501,9 @@
       <c r="C16" t="s">
         <v>31</v>
       </c>
+      <c r="D16" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="M16" t="s">
         <v>92</v>
       </c>
@@ -1497,8 +1512,14 @@
       <c r="A17" t="s">
         <v>15</v>
       </c>
+      <c r="B17" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="C17" t="s">
         <v>32</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="M17" t="s">
         <v>93</v>
@@ -1508,6 +1529,9 @@
       <c r="C18" t="s">
         <v>33</v>
       </c>
+      <c r="D18" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="M18" t="s">
         <v>94</v>
       </c>
@@ -1516,45 +1540,72 @@
       <c r="C19" t="s">
         <v>34</v>
       </c>
+      <c r="D19" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>35</v>
       </c>
+      <c r="D20" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
         <v>36</v>
       </c>
+      <c r="D21" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
         <v>37</v>
       </c>
+      <c r="D22" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
         <v>38</v>
       </c>
+      <c r="D23" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
         <v>39</v>
       </c>
+      <c r="D24" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C25" t="s">
         <v>40</v>
       </c>
+      <c r="D25" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
         <v>41</v>
       </c>
+      <c r="D26" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C27" t="s">
         <v>42</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Implmented PdfPageObjects, and built out support for loading standard and embedded fonts. Also stubbed several PdfPageObject types. Added methods to add new text objects and manipulate them.
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\coding\dotPDFium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27A5535-F3BD-4560-9C2F-5AE5695165EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A330109-9A4A-4261-B101-9B0734ED6ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39090" yWindow="580" windowWidth="29750" windowHeight="15370" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
+    <workbookView xWindow="39090" yWindow="580" windowWidth="33140" windowHeight="15370" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="204">
   <si>
     <t>Text_LoadPage</t>
   </si>
@@ -642,6 +642,12 @@
   </si>
   <si>
     <t>xx</t>
+  </si>
+  <si>
+    <t>PageObj_GetType</t>
+  </si>
+  <si>
+    <t>Text_LoadFont</t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1052,7 @@
   <dimension ref="A1:R66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1102,6 +1108,9 @@
       <c r="O1" t="s">
         <v>95</v>
       </c>
+      <c r="P1" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="Q1" t="s">
         <v>110</v>
       </c>
@@ -1137,6 +1146,9 @@
       <c r="O2" t="s">
         <v>96</v>
       </c>
+      <c r="P2" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="Q2" t="s">
         <v>111</v>
       </c>
@@ -1169,6 +1181,9 @@
       <c r="O3" t="s">
         <v>97</v>
       </c>
+      <c r="P3" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="Q3" t="s">
         <v>112</v>
       </c>
@@ -1201,6 +1216,9 @@
       <c r="O4" t="s">
         <v>98</v>
       </c>
+      <c r="P4" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="Q4" t="s">
         <v>113</v>
       </c>
@@ -1233,6 +1251,9 @@
       <c r="O5" t="s">
         <v>99</v>
       </c>
+      <c r="P5" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="Q5" t="s">
         <v>114</v>
       </c>
@@ -1265,6 +1286,9 @@
       <c r="O6" t="s">
         <v>100</v>
       </c>
+      <c r="P6" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="Q6" t="s">
         <v>115</v>
       </c>
@@ -1404,6 +1428,9 @@
       <c r="O11" t="s">
         <v>105</v>
       </c>
+      <c r="P11" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -1430,6 +1457,9 @@
       <c r="O12" t="s">
         <v>106</v>
       </c>
+      <c r="P12" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1450,6 +1480,9 @@
       <c r="O13" t="s">
         <v>107</v>
       </c>
+      <c r="P13" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -1470,6 +1503,9 @@
       <c r="O14" t="s">
         <v>108</v>
       </c>
+      <c r="P14" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -1490,6 +1526,9 @@
       <c r="O15" t="s">
         <v>109</v>
       </c>
+      <c r="P15" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -1507,6 +1546,12 @@
       <c r="M16" t="s">
         <v>92</v>
       </c>
+      <c r="O16" t="s">
+        <v>202</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
@@ -1524,6 +1569,12 @@
       <c r="M17" t="s">
         <v>93</v>
       </c>
+      <c r="O17" t="s">
+        <v>203</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
@@ -1609,6 +1660,7 @@
       </c>
     </row>
     <row r="28" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="1"/>
       <c r="B28" s="3"/>
       <c r="C28" s="1"/>
       <c r="D28" s="3"/>
@@ -1643,6 +1695,9 @@
       <c r="I30" t="s">
         <v>143</v>
       </c>
+      <c r="J30" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="K30" t="s">
         <v>145</v>
       </c>
@@ -1665,6 +1720,9 @@
       </c>
       <c r="I31" t="s">
         <v>144</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="K31" t="s">
         <v>146</v>

</xml_diff>

<commit_message>
Fixed save file struct and writer delegate
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\coding\dotPDFium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A330109-9A4A-4261-B101-9B0734ED6ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E3F072-57B9-4643-8EEE-E2416F8F241B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39090" yWindow="580" windowWidth="33140" windowHeight="15370" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
+    <workbookView xWindow="3430" yWindow="2210" windowWidth="33140" windowHeight="15370" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Audit of native functions; added most missing functions.
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\coding\dotPDFium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E3F072-57B9-4643-8EEE-E2416F8F241B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA964E80-7F51-4ECC-A4C1-42A13BB88FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3430" yWindow="2210" windowWidth="33140" windowHeight="15370" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
+    <workbookView xWindow="3770" yWindow="2550" windowWidth="33140" windowHeight="15370" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>

<commit_message>
Separated enums into PdfEnums.cs file.
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\coding\dotPDFium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA964E80-7F51-4ECC-A4C1-42A13BB88FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E8DC2B-F407-40EE-BDD4-12B86A10DC66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3770" yWindow="2550" windowWidth="33140" windowHeight="15370" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
+    <workbookView xWindow="3430" yWindow="2210" windowWidth="33140" windowHeight="15370" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="212">
   <si>
     <t>Text_LoadPage</t>
   </si>
@@ -649,6 +648,30 @@
   </si>
   <si>
     <t>Text_LoadFont</t>
+  </si>
+  <si>
+    <t>Page_HasTransparency</t>
+  </si>
+  <si>
+    <t>PageObj_GetIsActive</t>
+  </si>
+  <si>
+    <t>PageObj_SetIsActive</t>
+  </si>
+  <si>
+    <t>PageObjTransformF</t>
+  </si>
+  <si>
+    <t>PageObj_GetMatrix</t>
+  </si>
+  <si>
+    <t>PageObj_SetMatrix</t>
+  </si>
+  <si>
+    <t>Page_TransformAnnots</t>
+  </si>
+  <si>
+    <t>PageObj_NewImageObj</t>
   </si>
 </sst>
 </file>
@@ -1053,7 +1076,7 @@
   <dimension ref="A1:R66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1322,6 +1345,9 @@
       <c r="O7" t="s">
         <v>101</v>
       </c>
+      <c r="P7" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -1377,6 +1403,9 @@
       <c r="O9" t="s">
         <v>103</v>
       </c>
+      <c r="P9" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -1403,6 +1432,9 @@
       <c r="O10" t="s">
         <v>104</v>
       </c>
+      <c r="P10" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -1587,6 +1619,9 @@
       <c r="M18" t="s">
         <v>94</v>
       </c>
+      <c r="O18" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
@@ -1595,6 +1630,9 @@
       <c r="D19" s="2" t="s">
         <v>199</v>
       </c>
+      <c r="O19" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
@@ -1603,6 +1641,9 @@
       <c r="D20" s="2" t="s">
         <v>199</v>
       </c>
+      <c r="O20" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
@@ -1611,6 +1652,9 @@
       <c r="D21" s="2" t="s">
         <v>199</v>
       </c>
+      <c r="O21" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
@@ -1619,6 +1663,9 @@
       <c r="D22" s="2" t="s">
         <v>199</v>
       </c>
+      <c r="O22" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
@@ -1627,6 +1674,9 @@
       <c r="D23" s="2" t="s">
         <v>199</v>
       </c>
+      <c r="O23" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
@@ -1635,6 +1685,9 @@
       <c r="D24" s="2" t="s">
         <v>199</v>
       </c>
+      <c r="O24" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C25" t="s">
@@ -1643,6 +1696,9 @@
       <c r="D25" s="2" t="s">
         <v>199</v>
       </c>
+      <c r="O25" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
@@ -1650,6 +1706,9 @@
       </c>
       <c r="D26" s="2" t="s">
         <v>199</v>
+      </c>
+      <c r="O26" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Working on further building out the API
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\coding\dotPDFium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8625659-B7F6-42E9-8A7B-623D8DB5E9C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C2FA43-949B-4EDF-A8FD-A52B54FDDCA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39880" yWindow="270" windowWidth="23310" windowHeight="19510" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
+    <workbookView xWindow="40220" yWindow="610" windowWidth="36190" windowHeight="19510" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1245,7 +1245,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1255,6 +1255,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -1320,10 +1327,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1347,12 +1355,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1686,14 +1702,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93991F7-7A9D-4291-8EC0-AB472EBDEDBD}">
   <dimension ref="A1:R101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.90625" customWidth="1"/>
-    <col min="2" max="2" width="3.90625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.36328125" style="2" customWidth="1"/>
     <col min="3" max="3" width="36.08984375" customWidth="1"/>
     <col min="4" max="4" width="4" style="2" customWidth="1"/>
     <col min="5" max="5" width="25.90625" customWidth="1"/>
@@ -2182,6 +2198,9 @@
       <c r="A17" t="s">
         <v>285</v>
       </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
       <c r="C17" t="s">
         <v>299</v>
       </c>
@@ -2250,6 +2269,9 @@
       <c r="A21" t="s">
         <v>283</v>
       </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
       <c r="C21" t="s">
         <v>312</v>
       </c>
@@ -2264,8 +2286,14 @@
       <c r="A22" t="s">
         <v>281</v>
       </c>
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
       <c r="C22" t="s">
         <v>301</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1</v>
       </c>
       <c r="M22" t="s">
         <v>330</v>
@@ -2278,6 +2306,9 @@
       <c r="A23" t="s">
         <v>280</v>
       </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
       <c r="C23" t="s">
         <v>22</v>
       </c>
@@ -2295,6 +2326,9 @@
       <c r="A24" t="s">
         <v>282</v>
       </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
       <c r="C24" t="s">
         <v>26</v>
       </c>
@@ -2312,6 +2346,9 @@
       <c r="A25" t="s">
         <v>286</v>
       </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
       <c r="C25" t="s">
         <v>28</v>
       </c>
@@ -2329,8 +2366,14 @@
       <c r="A26" t="s">
         <v>287</v>
       </c>
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
       <c r="C26" t="s">
         <v>303</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1</v>
       </c>
       <c r="M26" t="s">
         <v>329</v>
@@ -2348,6 +2391,9 @@
       </c>
       <c r="C27" t="s">
         <v>302</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1</v>
       </c>
       <c r="M27" t="s">
         <v>93</v>
@@ -2419,6 +2465,9 @@
       <c r="A30" t="s">
         <v>284</v>
       </c>
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
       <c r="C30" t="s">
         <v>300</v>
       </c>
@@ -2490,6 +2539,9 @@
       <c r="A32" t="s">
         <v>276</v>
       </c>
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
       <c r="C32" t="s">
         <v>316</v>
       </c>
@@ -2565,6 +2617,9 @@
       <c r="A34" t="s">
         <v>279</v>
       </c>
+      <c r="B34" s="2">
+        <v>1</v>
+      </c>
       <c r="C34" t="s">
         <v>315</v>
       </c>
@@ -2591,6 +2646,9 @@
       <c r="A35" t="s">
         <v>277</v>
       </c>
+      <c r="B35" s="2">
+        <v>1</v>
+      </c>
       <c r="C35" t="s">
         <v>16</v>
       </c>
@@ -2621,8 +2679,14 @@
       <c r="A36" t="s">
         <v>278</v>
       </c>
+      <c r="B36" s="2">
+        <v>1</v>
+      </c>
       <c r="C36" t="s">
         <v>295</v>
+      </c>
+      <c r="D36" s="2">
+        <v>1</v>
       </c>
       <c r="E36" t="s">
         <v>130</v>
@@ -2669,7 +2733,7 @@
       </c>
       <c r="B38" s="2">
         <f>SUM(B2:B37)</f>
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C38" t="s">
         <v>19</v>
@@ -2839,10 +2903,6 @@
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A48" s="11" t="s">
-        <v>399</v>
-      </c>
-      <c r="B48" s="11"/>
       <c r="C48" t="s">
         <v>307</v>
       </c>
@@ -2869,13 +2929,6 @@
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A49" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="B49" s="9">
-        <f>A38</f>
-        <v>36</v>
-      </c>
       <c r="C49" t="s">
         <v>308</v>
       </c>
@@ -2902,13 +2955,6 @@
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A50" s="10" t="s">
-        <v>317</v>
-      </c>
-      <c r="B50" s="9">
-        <f>C51</f>
-        <v>50</v>
-      </c>
       <c r="C50" t="s">
         <v>304</v>
       </c>
@@ -2939,19 +2985,12 @@
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A51" s="10" t="s">
-        <v>319</v>
-      </c>
-      <c r="B51" s="9">
-        <f>E14</f>
-        <v>12</v>
-      </c>
       <c r="C51" s="4">
         <v>50</v>
       </c>
       <c r="D51" s="2">
         <f>SUM(D2:D50)</f>
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E51" t="s">
         <v>185</v>
@@ -2973,13 +3012,6 @@
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A52" s="10" t="s">
-        <v>320</v>
-      </c>
-      <c r="B52" s="9">
-        <f>G15</f>
-        <v>13</v>
-      </c>
       <c r="E52" t="s">
         <v>186</v>
       </c>
@@ -3004,13 +3036,11 @@
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A53" s="10" t="s">
-        <v>321</v>
-      </c>
-      <c r="B53" s="9">
-        <f>I4</f>
-        <v>2</v>
-      </c>
+      <c r="A53" s="11" t="s">
+        <v>399</v>
+      </c>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
       <c r="E53" t="s">
         <v>187</v>
       </c>
@@ -3029,11 +3059,15 @@
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A54" s="10" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B54" s="9">
-        <f>K10</f>
-        <v>8</v>
+        <f>A38</f>
+        <v>36</v>
+      </c>
+      <c r="C54" s="12">
+        <f>B38</f>
+        <v>29</v>
       </c>
       <c r="E54" t="s">
         <v>181</v>
@@ -3053,11 +3087,15 @@
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A55" s="10" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B55" s="9">
-        <f>M31</f>
-        <v>29</v>
+        <f>C51</f>
+        <v>50</v>
+      </c>
+      <c r="C55" s="12">
+        <f>D51</f>
+        <v>31</v>
       </c>
       <c r="E55" t="s">
         <v>179</v>
@@ -3077,11 +3115,15 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A56" s="10" t="s">
-        <v>400</v>
+        <v>319</v>
       </c>
       <c r="B56" s="9">
-        <f>O101</f>
-        <v>99</v>
+        <f>E14</f>
+        <v>12</v>
+      </c>
+      <c r="C56" s="12">
+        <f>F14</f>
+        <v>0</v>
       </c>
       <c r="E56" t="s">
         <v>178</v>
@@ -3105,11 +3147,15 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A57" s="10" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B57" s="9">
-        <f>Q8</f>
-        <v>6</v>
+        <f>G15</f>
+        <v>13</v>
+      </c>
+      <c r="C57" s="12">
+        <f>H15</f>
+        <v>0</v>
       </c>
       <c r="E57" t="s">
         <v>177</v>
@@ -3129,11 +3175,15 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A58" s="10" t="s">
-        <v>374</v>
+        <v>321</v>
       </c>
       <c r="B58" s="9">
-        <f>E38</f>
-        <v>7</v>
+        <f>I4</f>
+        <v>2</v>
+      </c>
+      <c r="C58" s="12">
+        <f>J4</f>
+        <v>0</v>
       </c>
       <c r="E58" t="s">
         <v>180</v>
@@ -3150,11 +3200,15 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A59" s="10" t="s">
-        <v>375</v>
+        <v>323</v>
       </c>
       <c r="B59" s="9">
-        <f>G35</f>
-        <v>4</v>
+        <f>K10</f>
+        <v>8</v>
+      </c>
+      <c r="C59" s="12">
+        <f>L10</f>
+        <v>0</v>
       </c>
       <c r="E59" t="s">
         <v>190</v>
@@ -3171,11 +3225,15 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A60" s="10" t="s">
-        <v>376</v>
+        <v>322</v>
       </c>
       <c r="B60" s="9">
-        <f>I33</f>
-        <v>2</v>
+        <f>M31</f>
+        <v>29</v>
+      </c>
+      <c r="C60" s="12">
+        <f>N31</f>
+        <v>0</v>
       </c>
       <c r="E60" t="s">
         <v>176</v>
@@ -3195,11 +3253,15 @@
     </row>
     <row r="61" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="10" t="s">
-        <v>377</v>
+        <v>400</v>
       </c>
       <c r="B61" s="9">
-        <f>K33</f>
-        <v>2</v>
+        <f>O101</f>
+        <v>99</v>
+      </c>
+      <c r="C61" s="12">
+        <f>P101</f>
+        <v>17</v>
       </c>
       <c r="E61" t="s">
         <v>174</v>
@@ -3220,119 +3282,147 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A62" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="B62" s="9">
+        <f>Q8</f>
+        <v>6</v>
+      </c>
+      <c r="C62" s="12">
+        <f>R8</f>
+        <v>0</v>
+      </c>
+      <c r="E62" t="s">
+        <v>173</v>
+      </c>
+      <c r="I62" t="s">
+        <v>366</v>
+      </c>
+      <c r="O62" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A63" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="B63" s="9">
+        <f>E38</f>
+        <v>7</v>
+      </c>
+      <c r="C63" s="12">
+        <f>F38</f>
+        <v>0</v>
+      </c>
+      <c r="E63" t="s">
+        <v>172</v>
+      </c>
+      <c r="I63" t="s">
+        <v>356</v>
+      </c>
+      <c r="O63" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A64" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="B64" s="9">
+        <f>G35</f>
+        <v>4</v>
+      </c>
+      <c r="C64" s="12">
+        <f>H35</f>
+        <v>0</v>
+      </c>
+      <c r="E64" t="s">
+        <v>175</v>
+      </c>
+      <c r="I64" t="s">
+        <v>357</v>
+      </c>
+      <c r="O64" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A65" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="B65" s="9">
+        <f>I33</f>
+        <v>2</v>
+      </c>
+      <c r="C65" s="12">
+        <f>J33</f>
+        <v>2</v>
+      </c>
+      <c r="E65" t="s">
+        <v>182</v>
+      </c>
+      <c r="I65" t="s">
+        <v>373</v>
+      </c>
+      <c r="O65" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A66" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="B66" s="9">
+        <f>K33</f>
+        <v>2</v>
+      </c>
+      <c r="C66" s="12">
+        <f>L33</f>
+        <v>0</v>
+      </c>
+      <c r="E66" t="s">
+        <v>184</v>
+      </c>
+      <c r="I66" t="s">
+        <v>340</v>
+      </c>
+      <c r="O66" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A67" s="10" t="s">
         <v>378</v>
       </c>
-      <c r="B62" s="9">
+      <c r="B67" s="9">
         <f>M41</f>
         <v>8</v>
       </c>
-      <c r="E62" t="s">
-        <v>173</v>
-      </c>
-      <c r="I62" t="s">
-        <v>366</v>
-      </c>
-      <c r="O62" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A63" s="10" t="s">
+      <c r="C67" s="12">
+        <f>N41</f>
+        <v>0</v>
+      </c>
+      <c r="E67" t="s">
+        <v>183</v>
+      </c>
+      <c r="I67" t="s">
+        <v>119</v>
+      </c>
+      <c r="O67" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A68" s="10" t="s">
         <v>379</v>
       </c>
-      <c r="B63" s="9">
+      <c r="B68" s="9">
         <f>Q61</f>
         <v>29</v>
       </c>
-      <c r="E63" t="s">
-        <v>172</v>
-      </c>
-      <c r="I63" t="s">
-        <v>356</v>
-      </c>
-      <c r="O63" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A64" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="B64" s="9">
-        <f>E68</f>
-        <v>20</v>
-      </c>
-      <c r="E64" t="s">
-        <v>175</v>
-      </c>
-      <c r="I64" t="s">
-        <v>357</v>
-      </c>
-      <c r="O64" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A65" s="10" t="s">
-        <v>397</v>
-      </c>
-      <c r="B65" s="9">
-        <f>G52</f>
-        <v>3</v>
-      </c>
-      <c r="E65" t="s">
-        <v>182</v>
-      </c>
-      <c r="I65" t="s">
-        <v>373</v>
-      </c>
-      <c r="O65" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A66" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="B66" s="9">
-        <f>I91</f>
-        <v>42</v>
-      </c>
-      <c r="E66" t="s">
-        <v>184</v>
-      </c>
-      <c r="I66" t="s">
-        <v>340</v>
-      </c>
-      <c r="O66" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A67" s="10" t="s">
-        <v>326</v>
-      </c>
-      <c r="B67" s="9">
-        <f>K50</f>
-        <v>1</v>
-      </c>
-      <c r="E67" t="s">
-        <v>183</v>
-      </c>
-      <c r="I67" t="s">
-        <v>119</v>
-      </c>
-      <c r="O67" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A68" s="10" t="s">
-        <v>395</v>
-      </c>
-      <c r="B68" s="9">
-        <f>M56</f>
-        <v>7</v>
+      <c r="C68" s="12">
+        <f>R61</f>
+        <v>0</v>
       </c>
       <c r="E68" s="4">
         <v>20</v>
@@ -3349,8 +3439,17 @@
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A69" s="10"/>
-      <c r="B69" s="9"/>
+      <c r="A69" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="B69" s="9">
+        <f>E68</f>
+        <v>20</v>
+      </c>
+      <c r="C69" s="12">
+        <f>F68</f>
+        <v>0</v>
+      </c>
       <c r="I69" t="s">
         <v>346</v>
       </c>
@@ -3359,10 +3458,16 @@
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A70" s="10"/>
+      <c r="A70" s="10" t="s">
+        <v>397</v>
+      </c>
       <c r="B70" s="9">
-        <f>SUM(B52:B69)</f>
-        <v>282</v>
+        <f>G52</f>
+        <v>3</v>
+      </c>
+      <c r="C70" s="12">
+        <f>H52</f>
+        <v>0</v>
       </c>
       <c r="I70" t="s">
         <v>344</v>
@@ -3372,6 +3477,17 @@
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A71" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="B71" s="9">
+        <f>I91</f>
+        <v>42</v>
+      </c>
+      <c r="C71" s="12">
+        <f>J91</f>
+        <v>0</v>
+      </c>
       <c r="I71" t="s">
         <v>347</v>
       </c>
@@ -3383,6 +3499,17 @@
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A72" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="B72" s="9">
+        <f>K50</f>
+        <v>1</v>
+      </c>
+      <c r="C72" s="12">
+        <f>L50</f>
+        <v>0</v>
+      </c>
       <c r="I72" t="s">
         <v>348</v>
       </c>
@@ -3394,6 +3521,17 @@
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A73" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="B73" s="9">
+        <f>M56</f>
+        <v>7</v>
+      </c>
+      <c r="C73" s="12">
+        <f>N56</f>
+        <v>0</v>
+      </c>
       <c r="I73" t="s">
         <v>355</v>
       </c>
@@ -3402,6 +3540,9 @@
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A74" s="10"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="12"/>
       <c r="I74" t="s">
         <v>351</v>
       </c>
@@ -3410,6 +3551,15 @@
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A75" s="10"/>
+      <c r="B75" s="9">
+        <f>SUM(B54:B74)</f>
+        <v>380</v>
+      </c>
+      <c r="C75" s="12">
+        <f>SUM(C54:C74)</f>
+        <v>79</v>
+      </c>
       <c r="I75" t="s">
         <v>352</v>
       </c>
@@ -3418,6 +3568,12 @@
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A76" s="13"/>
+      <c r="B76" s="14">
+        <f>C75/B75</f>
+        <v>0.20789473684210527</v>
+      </c>
+      <c r="C76" s="13"/>
       <c r="I76" t="s">
         <v>353</v>
       </c>
@@ -3617,7 +3773,7 @@
     <sortCondition ref="M49:M55"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A53:C53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Worked on implementing the build out of the PdfPageObjects- Text, Image and Path.
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\coding\dotPDFium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C2FA43-949B-4EDF-A8FD-A52B54FDDCA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9369298B-1101-4F31-843F-DC5C7CA224AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40220" yWindow="610" windowWidth="36190" windowHeight="19510" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="399">
   <si>
     <t>Text_LoadPage</t>
   </si>
@@ -629,9 +629,6 @@
     <t>PageObj_SetIsActive</t>
   </si>
   <si>
-    <t>PageObjTransformF</t>
-  </si>
-  <si>
     <t>PageObj_GetMatrix</t>
   </si>
   <si>
@@ -696,9 +693,6 @@
   </si>
   <si>
     <t>Path_GetDrawMode</t>
-  </si>
-  <si>
-    <t>Path_SetCharcodes</t>
   </si>
   <si>
     <t>Text_LoadCidType2Font</t>
@@ -1355,15 +1349,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1700,10 +1694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93991F7-7A9D-4291-8EC0-AB472EBDEDBD}">
-  <dimension ref="A1:R101"/>
+  <dimension ref="A1:R99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1730,36 +1724,36 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="K1" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="K1" s="5" t="s">
+      <c r="O1" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>323</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -1783,7 +1777,7 @@
         <v>89</v>
       </c>
       <c r="O2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="Q2" t="s">
         <v>113</v>
@@ -1791,7 +1785,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
@@ -1803,7 +1797,7 @@
         <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="I3" t="s">
         <v>68</v>
@@ -1826,7 +1820,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C4" t="s">
         <v>31</v>
@@ -1865,7 +1859,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
@@ -1886,7 +1880,7 @@
         <v>86</v>
       </c>
       <c r="O5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="Q5" t="s">
         <v>111</v>
@@ -1894,7 +1888,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C6" t="s">
         <v>32</v>
@@ -1915,7 +1909,7 @@
         <v>84</v>
       </c>
       <c r="O6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="Q6" t="s">
         <v>110</v>
@@ -1923,7 +1917,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C7" t="s">
         <v>36</v>
@@ -1944,7 +1938,7 @@
         <v>87</v>
       </c>
       <c r="O7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="Q7" t="s">
         <v>114</v>
@@ -1952,7 +1946,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C8" t="s">
         <v>34</v>
@@ -1973,7 +1967,7 @@
         <v>83</v>
       </c>
       <c r="O8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="Q8" s="4">
         <v>6</v>
@@ -2009,7 +2003,7 @@
         <v>81</v>
       </c>
       <c r="O9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
@@ -2042,7 +2036,7 @@
         <v>82</v>
       </c>
       <c r="O10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
@@ -2068,7 +2062,7 @@
         <v>80</v>
       </c>
       <c r="O11" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
@@ -2094,7 +2088,7 @@
         <v>77</v>
       </c>
       <c r="O12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
@@ -2105,7 +2099,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E13" t="s">
         <v>49</v>
@@ -2117,7 +2111,7 @@
         <v>78</v>
       </c>
       <c r="O13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
@@ -2147,7 +2141,7 @@
         <v>79</v>
       </c>
       <c r="O14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
@@ -2174,7 +2168,7 @@
         <v>88</v>
       </c>
       <c r="O15" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
@@ -2185,30 +2179,30 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="M16" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O16" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="M17" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="O17" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
@@ -2219,13 +2213,13 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="M18" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="O18" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.35">
@@ -2242,10 +2236,10 @@
         <v>1</v>
       </c>
       <c r="M19" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O19" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
@@ -2256,55 +2250,64 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="M20" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="O20" t="s">
-        <v>264</v>
+        <v>262</v>
+      </c>
+      <c r="P20" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B21" s="2">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="M21" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O21" t="s">
-        <v>258</v>
+        <v>256</v>
+      </c>
+      <c r="P21" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B22" s="2">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D22" s="2">
         <v>1</v>
       </c>
       <c r="M22" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="O22" t="s">
-        <v>259</v>
+        <v>257</v>
+      </c>
+      <c r="P22" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B23" s="2">
         <v>1</v>
@@ -2316,15 +2319,18 @@
         <v>1</v>
       </c>
       <c r="M23" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="O23" t="s">
-        <v>261</v>
+        <v>259</v>
+      </c>
+      <c r="P23" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B24" s="2">
         <v>1</v>
@@ -2339,12 +2345,15 @@
         <v>94</v>
       </c>
       <c r="O24" t="s">
-        <v>260</v>
+        <v>258</v>
+      </c>
+      <c r="P24" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B25" s="2">
         <v>1</v>
@@ -2356,30 +2365,36 @@
         <v>1</v>
       </c>
       <c r="M25" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="O25" t="s">
-        <v>262</v>
+        <v>260</v>
+      </c>
+      <c r="P25" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D26" s="2">
         <v>1</v>
       </c>
       <c r="M26" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="O26" t="s">
-        <v>263</v>
+        <v>261</v>
+      </c>
+      <c r="P26" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.35">
@@ -2390,7 +2405,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D27" s="2">
         <v>1</v>
@@ -2463,28 +2478,28 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B30" s="2">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E30" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="I30" s="6" t="s">
         <v>374</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="K30" s="6" t="s">
         <v>375</v>
       </c>
-      <c r="I30" s="6" t="s">
-        <v>376</v>
-      </c>
-      <c r="K30" s="6" t="s">
-        <v>377</v>
-      </c>
       <c r="M30" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="O30" t="s">
         <v>101</v>
@@ -2493,7 +2508,7 @@
         <v>1</v>
       </c>
       <c r="Q30" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2504,7 +2519,7 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E31" t="s">
         <v>129</v>
@@ -2529,21 +2544,24 @@
         <v>0</v>
       </c>
       <c r="O31" t="s">
-        <v>202</v>
+        <v>201</v>
+      </c>
+      <c r="P31" s="2">
+        <v>1</v>
       </c>
       <c r="Q31" s="7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B32" s="2">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E32" t="s">
         <v>131</v>
@@ -2561,13 +2579,16 @@
         <v>139</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="O32" t="s">
         <v>194</v>
       </c>
+      <c r="P32" s="2">
+        <v>1</v>
+      </c>
       <c r="Q32" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
@@ -2578,7 +2599,7 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E33" t="s">
         <v>127</v>
@@ -2610,18 +2631,18 @@
         <v>1</v>
       </c>
       <c r="Q33" s="7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B34" s="2">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E34" t="s">
         <v>126</v>
@@ -2639,12 +2660,12 @@
         <v>1</v>
       </c>
       <c r="Q34" s="7" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B35" s="2">
         <v>1</v>
@@ -2669,21 +2690,24 @@
         <v>143</v>
       </c>
       <c r="O35" t="s">
-        <v>204</v>
+        <v>203</v>
+      </c>
+      <c r="P35" s="2">
+        <v>1</v>
       </c>
       <c r="Q35" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B36" s="2">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D36" s="2">
         <v>1</v>
@@ -2695,10 +2719,13 @@
         <v>142</v>
       </c>
       <c r="O36" t="s">
-        <v>203</v>
+        <v>202</v>
+      </c>
+      <c r="P36" s="2">
+        <v>1</v>
       </c>
       <c r="Q36" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
@@ -2721,10 +2748,10 @@
         <v>147</v>
       </c>
       <c r="O37" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Q37" s="7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
@@ -2752,10 +2779,10 @@
         <v>145</v>
       </c>
       <c r="O38" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="Q38" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
@@ -2769,10 +2796,10 @@
         <v>144</v>
       </c>
       <c r="O39" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="Q39" s="7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
@@ -2786,10 +2813,13 @@
         <v>146</v>
       </c>
       <c r="O40" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="P40" s="2">
+        <v>1</v>
       </c>
       <c r="Q40" s="7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
@@ -2807,7 +2837,10 @@
         <v>0</v>
       </c>
       <c r="O41" t="s">
-        <v>214</v>
+        <v>213</v>
+      </c>
+      <c r="P41" s="2">
+        <v>1</v>
       </c>
       <c r="Q41" t="s">
         <v>152</v>
@@ -2840,13 +2873,16 @@
       <c r="O43" t="s">
         <v>102</v>
       </c>
+      <c r="P43" s="2">
+        <v>1</v>
+      </c>
       <c r="Q43" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C44" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="O44" t="s">
         <v>104</v>
@@ -2855,26 +2891,26 @@
         <v>1</v>
       </c>
       <c r="Q44" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C45" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="O45" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="Q45" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C46" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="O46" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="Q46" t="s">
         <v>154</v>
@@ -2884,7 +2920,7 @@
       <c r="A47" s="1"/>
       <c r="B47" s="3"/>
       <c r="C47" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="3"/>
@@ -2896,33 +2932,36 @@
       <c r="L47" s="3"/>
       <c r="M47" s="1"/>
       <c r="O47" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="Q47" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C48" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="O48" t="s">
-        <v>208</v>
+        <v>207</v>
+      </c>
+      <c r="P48" s="2">
+        <v>1</v>
       </c>
       <c r="Q48" t="s">
         <v>158</v>
@@ -2930,7 +2969,7 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C49" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E49" t="s">
         <v>188</v>
@@ -2950,13 +2989,16 @@
       <c r="O49" t="s">
         <v>195</v>
       </c>
+      <c r="P49" s="2">
+        <v>1</v>
+      </c>
       <c r="Q49" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C50" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E50" t="s">
         <v>189</v>
@@ -2978,7 +3020,7 @@
         <v>165</v>
       </c>
       <c r="O50" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="Q50" t="s">
         <v>155</v>
@@ -3005,10 +3047,10 @@
         <v>164</v>
       </c>
       <c r="O51" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Q51" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.35">
@@ -3029,18 +3071,18 @@
         <v>167</v>
       </c>
       <c r="O52" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="Q52" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A53" s="11" t="s">
-        <v>399</v>
-      </c>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
+      <c r="A53" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
       <c r="E53" t="s">
         <v>187</v>
       </c>
@@ -3051,7 +3093,10 @@
         <v>168</v>
       </c>
       <c r="O53" t="s">
-        <v>198</v>
+        <v>197</v>
+      </c>
+      <c r="P53" s="2">
+        <v>1</v>
       </c>
       <c r="Q53" t="s">
         <v>153</v>
@@ -3059,13 +3104,13 @@
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A54" s="10" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B54" s="9">
         <f>A38</f>
         <v>36</v>
       </c>
-      <c r="C54" s="12">
+      <c r="C54" s="11">
         <f>B38</f>
         <v>29</v>
       </c>
@@ -3073,27 +3118,30 @@
         <v>181</v>
       </c>
       <c r="I54" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="M54" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="O54" t="s">
-        <v>270</v>
+        <v>268</v>
+      </c>
+      <c r="P54" s="2">
+        <v>1</v>
       </c>
       <c r="Q54" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A55" s="10" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B55" s="9">
         <f>C51</f>
         <v>50</v>
       </c>
-      <c r="C55" s="12">
+      <c r="C55" s="11">
         <f>D51</f>
         <v>31</v>
       </c>
@@ -3101,13 +3149,16 @@
         <v>179</v>
       </c>
       <c r="I55" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="M55" t="s">
         <v>163</v>
       </c>
       <c r="O55" t="s">
-        <v>210</v>
+        <v>209</v>
+      </c>
+      <c r="P55" s="2">
+        <v>1</v>
       </c>
       <c r="Q55" t="s">
         <v>162</v>
@@ -3115,13 +3166,13 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A56" s="10" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B56" s="9">
         <f>E14</f>
         <v>12</v>
       </c>
-      <c r="C56" s="12">
+      <c r="C56" s="11">
         <f>F14</f>
         <v>0</v>
       </c>
@@ -3129,7 +3180,7 @@
         <v>178</v>
       </c>
       <c r="I56" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="M56" s="4">
         <v>7</v>
@@ -3139,7 +3190,10 @@
         <v>0</v>
       </c>
       <c r="O56" t="s">
-        <v>212</v>
+        <v>211</v>
+      </c>
+      <c r="P56" s="2">
+        <v>1</v>
       </c>
       <c r="Q56" t="s">
         <v>160</v>
@@ -3147,13 +3201,13 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A57" s="10" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B57" s="9">
         <f>G15</f>
         <v>13</v>
       </c>
-      <c r="C57" s="12">
+      <c r="C57" s="11">
         <f>H15</f>
         <v>0</v>
       </c>
@@ -3161,7 +3215,7 @@
         <v>177</v>
       </c>
       <c r="I57" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="O57" t="s">
         <v>192</v>
@@ -3175,13 +3229,13 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A58" s="10" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B58" s="9">
         <f>I4</f>
         <v>2</v>
       </c>
-      <c r="C58" s="12">
+      <c r="C58" s="11">
         <f>J4</f>
         <v>0</v>
       </c>
@@ -3192,7 +3246,10 @@
         <v>120</v>
       </c>
       <c r="O58" t="s">
-        <v>205</v>
+        <v>204</v>
+      </c>
+      <c r="P58" s="2">
+        <v>1</v>
       </c>
       <c r="Q58" t="s">
         <v>150</v>
@@ -3200,13 +3257,13 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A59" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B59" s="9">
         <f>K10</f>
         <v>8</v>
       </c>
-      <c r="C59" s="12">
+      <c r="C59" s="11">
         <f>L10</f>
         <v>0</v>
       </c>
@@ -3217,7 +3274,10 @@
         <v>121</v>
       </c>
       <c r="O59" t="s">
-        <v>201</v>
+        <v>200</v>
+      </c>
+      <c r="P59" s="2">
+        <v>1</v>
       </c>
       <c r="Q59" t="s">
         <v>151</v>
@@ -3225,13 +3285,13 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A60" s="10" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B60" s="9">
         <f>M31</f>
         <v>29</v>
       </c>
-      <c r="C60" s="12">
+      <c r="C60" s="11">
         <f>N31</f>
         <v>0</v>
       </c>
@@ -3239,7 +3299,7 @@
         <v>176</v>
       </c>
       <c r="I60" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="O60" t="s">
         <v>105</v>
@@ -3253,24 +3313,24 @@
     </row>
     <row r="61" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="10" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B61" s="9">
-        <f>O101</f>
-        <v>99</v>
-      </c>
-      <c r="C61" s="12">
-        <f>P101</f>
-        <v>17</v>
+        <f>O99</f>
+        <v>97</v>
+      </c>
+      <c r="C61" s="11">
+        <f>P99</f>
+        <v>56</v>
       </c>
       <c r="E61" t="s">
         <v>174</v>
       </c>
       <c r="I61" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="O61" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="Q61" s="8">
         <v>29</v>
@@ -3282,13 +3342,13 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A62" s="10" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B62" s="9">
         <f>Q8</f>
         <v>6</v>
       </c>
-      <c r="C62" s="12">
+      <c r="C62" s="11">
         <f>R8</f>
         <v>0</v>
       </c>
@@ -3296,21 +3356,21 @@
         <v>173</v>
       </c>
       <c r="I62" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="O62" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A63" s="10" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B63" s="9">
         <f>E38</f>
         <v>7</v>
       </c>
-      <c r="C63" s="12">
+      <c r="C63" s="11">
         <f>F38</f>
         <v>0</v>
       </c>
@@ -3318,21 +3378,21 @@
         <v>172</v>
       </c>
       <c r="I63" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="O63" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A64" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B64" s="9">
         <f>G35</f>
         <v>4</v>
       </c>
-      <c r="C64" s="12">
+      <c r="C64" s="11">
         <f>H35</f>
         <v>0</v>
       </c>
@@ -3340,21 +3400,24 @@
         <v>175</v>
       </c>
       <c r="I64" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="O64" t="s">
-        <v>207</v>
+        <v>206</v>
+      </c>
+      <c r="P64" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B65" s="9">
         <f>I33</f>
         <v>2</v>
       </c>
-      <c r="C65" s="12">
+      <c r="C65" s="11">
         <f>J33</f>
         <v>2</v>
       </c>
@@ -3362,21 +3425,24 @@
         <v>182</v>
       </c>
       <c r="I65" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="O65" t="s">
         <v>196</v>
       </c>
+      <c r="P65" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B66" s="9">
         <f>K33</f>
         <v>2</v>
       </c>
-      <c r="C66" s="12">
+      <c r="C66" s="11">
         <f>L33</f>
         <v>0</v>
       </c>
@@ -3384,21 +3450,21 @@
         <v>184</v>
       </c>
       <c r="I66" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="O66" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="10" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B67" s="9">
         <f>M41</f>
         <v>8</v>
       </c>
-      <c r="C67" s="12">
+      <c r="C67" s="11">
         <f>N41</f>
         <v>0</v>
       </c>
@@ -3409,18 +3475,18 @@
         <v>119</v>
       </c>
       <c r="O67" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="10" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B68" s="9">
         <f>Q61</f>
         <v>29</v>
       </c>
-      <c r="C68" s="12">
+      <c r="C68" s="11">
         <f>R61</f>
         <v>0</v>
       </c>
@@ -3432,64 +3498,73 @@
         <v>0</v>
       </c>
       <c r="I68" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="O68" t="s">
-        <v>199</v>
+        <v>198</v>
+      </c>
+      <c r="P68" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="10" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B69" s="9">
         <f>E68</f>
         <v>20</v>
       </c>
-      <c r="C69" s="12">
+      <c r="C69" s="11">
         <f>F68</f>
         <v>0</v>
       </c>
       <c r="I69" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="O69" t="s">
-        <v>209</v>
+        <v>208</v>
+      </c>
+      <c r="P69" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="10" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B70" s="9">
         <f>G52</f>
         <v>3</v>
       </c>
-      <c r="C70" s="12">
+      <c r="C70" s="11">
         <f>H52</f>
         <v>0</v>
       </c>
       <c r="I70" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="O70" t="s">
-        <v>211</v>
+        <v>210</v>
+      </c>
+      <c r="P70" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="10" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B71" s="9">
         <f>I91</f>
         <v>42</v>
       </c>
-      <c r="C71" s="12">
+      <c r="C71" s="11">
         <f>J91</f>
         <v>0</v>
       </c>
       <c r="I71" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="O71" t="s">
         <v>103</v>
@@ -3500,21 +3575,21 @@
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" s="10" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B72" s="9">
         <f>K50</f>
         <v>1</v>
       </c>
-      <c r="C72" s="12">
+      <c r="C72" s="11">
         <f>L50</f>
         <v>0</v>
       </c>
       <c r="I72" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="O72" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="P72" s="2">
         <v>1</v>
@@ -3522,175 +3597,196 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B73" s="9">
         <f>M56</f>
         <v>7</v>
       </c>
-      <c r="C73" s="12">
+      <c r="C73" s="11">
         <f>N56</f>
         <v>0</v>
       </c>
       <c r="I73" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="O73" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" s="10"/>
       <c r="B74" s="9"/>
-      <c r="C74" s="12"/>
+      <c r="C74" s="11"/>
       <c r="I74" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="O74" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" s="10"/>
       <c r="B75" s="9">
         <f>SUM(B54:B74)</f>
-        <v>380</v>
-      </c>
-      <c r="C75" s="12">
+        <v>378</v>
+      </c>
+      <c r="C75" s="11">
         <f>SUM(C54:C74)</f>
-        <v>79</v>
+        <v>118</v>
       </c>
       <c r="I75" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="O75" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A76" s="13"/>
-      <c r="B76" s="14">
+      <c r="A76" s="12"/>
+      <c r="B76" s="13">
         <f>C75/B75</f>
-        <v>0.20789473684210527</v>
-      </c>
-      <c r="C76" s="13"/>
+        <v>0.31216931216931215</v>
+      </c>
+      <c r="C76" s="12"/>
       <c r="I76" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="O76" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="I77" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="O77" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="I78" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="O78" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="I79" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="O79" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="I80" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="O80" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="81" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I81" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="O81" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="82" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I82" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="O82" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="83" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I83" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="O83" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="84" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I84" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="O84" t="s">
-        <v>197</v>
+        <v>216</v>
+      </c>
+      <c r="P84" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I85" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="O85" t="s">
-        <v>217</v>
+        <v>218</v>
+      </c>
+      <c r="P85" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I86" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="O86" t="s">
-        <v>219</v>
+        <v>215</v>
+      </c>
+      <c r="P86" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I87" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="O87" t="s">
-        <v>216</v>
+        <v>214</v>
+      </c>
+      <c r="P87" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I88" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="O88" t="s">
-        <v>215</v>
+        <v>217</v>
+      </c>
+      <c r="P88" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I89" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="O89" t="s">
-        <v>220</v>
+        <v>219</v>
+      </c>
+      <c r="P89" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I90" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="O90" t="s">
-        <v>218</v>
+        <v>193</v>
+      </c>
+      <c r="P90" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="9:16" x14ac:dyDescent="0.35">
@@ -3702,12 +3798,15 @@
         <v>0</v>
       </c>
       <c r="O91" t="s">
-        <v>221</v>
+        <v>107</v>
+      </c>
+      <c r="P91" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="9:16" x14ac:dyDescent="0.35">
       <c r="O92" t="s">
-        <v>193</v>
+        <v>106</v>
       </c>
       <c r="P92" s="2">
         <v>1</v>
@@ -3715,7 +3814,7 @@
     </row>
     <row r="93" spans="9:16" x14ac:dyDescent="0.35">
       <c r="O93" t="s">
-        <v>107</v>
+        <v>225</v>
       </c>
       <c r="P93" s="2">
         <v>1</v>
@@ -3723,7 +3822,7 @@
     </row>
     <row r="94" spans="9:16" x14ac:dyDescent="0.35">
       <c r="O94" t="s">
-        <v>106</v>
+        <v>220</v>
       </c>
       <c r="P94" s="2">
         <v>1</v>
@@ -3731,41 +3830,43 @@
     </row>
     <row r="95" spans="9:16" x14ac:dyDescent="0.35">
       <c r="O95" t="s">
-        <v>227</v>
+        <v>224</v>
+      </c>
+      <c r="P95" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="9:16" x14ac:dyDescent="0.35">
       <c r="O96" t="s">
-        <v>222</v>
+        <v>223</v>
+      </c>
+      <c r="P96" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O97" t="s">
-        <v>226</v>
+        <v>222</v>
+      </c>
+      <c r="P97" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O98" t="s">
-        <v>225</v>
+        <v>221</v>
+      </c>
+      <c r="P98" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="15:16" x14ac:dyDescent="0.35">
-      <c r="O99" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="100" spans="15:16" x14ac:dyDescent="0.35">
-      <c r="O100" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="101" spans="15:16" x14ac:dyDescent="0.35">
-      <c r="O101" s="4">
-        <v>99</v>
-      </c>
-      <c r="P101" s="2">
-        <f>SUM(P2:P100)</f>
-        <v>17</v>
+      <c r="O99" s="4">
+        <v>97</v>
+      </c>
+      <c r="P99" s="2">
+        <f>SUM(P2:P98)</f>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Font system implementation and some re-shuffling + tracker updates.
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\coding\dotPDFium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1972F8F1-ECE6-4149-95C4-688EFA470EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9684D9E2-44E7-4360-B22A-07EDD6FCD8FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39090" yWindow="870" windowWidth="36190" windowHeight="19510" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
   </bookViews>
@@ -1322,7 +1322,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1346,6 +1346,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1354,6 +1357,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1693,16 +1699,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93991F7-7A9D-4291-8EC0-AB472EBDEDBD}">
   <dimension ref="A1:R99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.90625" customWidth="1"/>
     <col min="2" max="2" width="7.36328125" style="2" customWidth="1"/>
     <col min="3" max="3" width="36.08984375" customWidth="1"/>
-    <col min="4" max="4" width="4" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.26953125" style="2" customWidth="1"/>
     <col min="5" max="5" width="25.90625" customWidth="1"/>
     <col min="6" max="6" width="3.81640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="37.1796875" customWidth="1"/>
@@ -3040,17 +3044,29 @@
       <c r="E49" t="s">
         <v>187</v>
       </c>
+      <c r="F49" s="2">
+        <v>1</v>
+      </c>
       <c r="G49" t="s">
         <v>168</v>
       </c>
+      <c r="H49" s="2">
+        <v>1</v>
+      </c>
       <c r="I49" t="s">
         <v>121</v>
       </c>
       <c r="K49" t="s">
         <v>115</v>
       </c>
+      <c r="L49" s="2">
+        <v>1</v>
+      </c>
       <c r="M49" t="s">
         <v>165</v>
+      </c>
+      <c r="N49" s="2">
+        <v>1</v>
       </c>
       <c r="O49" t="s">
         <v>194</v>
@@ -3069,9 +3085,15 @@
       <c r="E50" t="s">
         <v>188</v>
       </c>
+      <c r="F50" s="2">
+        <v>1</v>
+      </c>
       <c r="G50" t="s">
         <v>169</v>
       </c>
+      <c r="H50" s="2">
+        <v>1</v>
+      </c>
       <c r="I50" t="s">
         <v>122</v>
       </c>
@@ -3080,10 +3102,13 @@
       </c>
       <c r="L50" s="2">
         <f>SUM(L49)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M50" t="s">
         <v>164</v>
+      </c>
+      <c r="N50" s="2">
+        <v>1</v>
       </c>
       <c r="O50" t="s">
         <v>271</v>
@@ -3103,14 +3128,23 @@
       <c r="E51" t="s">
         <v>184</v>
       </c>
+      <c r="F51" s="2">
+        <v>1</v>
+      </c>
       <c r="G51" t="s">
         <v>170</v>
       </c>
+      <c r="H51" s="2">
+        <v>1</v>
+      </c>
       <c r="I51" t="s">
         <v>123</v>
       </c>
       <c r="M51" t="s">
         <v>163</v>
+      </c>
+      <c r="N51" s="2">
+        <v>1</v>
       </c>
       <c r="O51" t="s">
         <v>269</v>
@@ -3123,12 +3157,15 @@
       <c r="E52" t="s">
         <v>185</v>
       </c>
+      <c r="F52" s="2">
+        <v>1</v>
+      </c>
       <c r="G52" s="4">
         <v>3</v>
       </c>
       <c r="H52" s="2">
         <f>SUM(H49:H51)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I52" t="s">
         <v>117</v>
@@ -3136,6 +3173,9 @@
       <c r="M52" t="s">
         <v>166</v>
       </c>
+      <c r="N52" s="2">
+        <v>1</v>
+      </c>
       <c r="O52" t="s">
         <v>241</v>
       </c>
@@ -3144,19 +3184,26 @@
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A53" s="14" t="s">
+      <c r="A53" s="15" t="s">
         <v>395</v>
       </c>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="11"/>
       <c r="E53" t="s">
         <v>186</v>
       </c>
+      <c r="F53" s="2">
+        <v>1</v>
+      </c>
       <c r="I53" t="s">
         <v>116</v>
       </c>
       <c r="M53" t="s">
         <v>167</v>
+      </c>
+      <c r="N53" s="2">
+        <v>1</v>
       </c>
       <c r="O53" t="s">
         <v>196</v>
@@ -3176,18 +3223,28 @@
         <f>A38</f>
         <v>36</v>
       </c>
-      <c r="C54" s="11">
+      <c r="C54" s="12">
         <f>B38</f>
         <v>29</v>
       </c>
+      <c r="D54" s="16">
+        <f>C54/B54</f>
+        <v>0.80555555555555558</v>
+      </c>
       <c r="E54" t="s">
         <v>180</v>
       </c>
+      <c r="F54" s="2">
+        <v>1</v>
+      </c>
       <c r="I54" t="s">
         <v>337</v>
       </c>
       <c r="M54" t="s">
         <v>392</v>
+      </c>
+      <c r="N54" s="2">
+        <v>1</v>
       </c>
       <c r="O54" t="s">
         <v>267</v>
@@ -3207,18 +3264,28 @@
         <f>C51</f>
         <v>50</v>
       </c>
-      <c r="C55" s="11">
+      <c r="C55" s="12">
         <f>D51</f>
         <v>31</v>
       </c>
+      <c r="D55" s="16">
+        <f t="shared" ref="D55:D73" si="0">C55/B55</f>
+        <v>0.62</v>
+      </c>
       <c r="E55" t="s">
         <v>178</v>
       </c>
+      <c r="F55" s="2">
+        <v>1</v>
+      </c>
       <c r="I55" t="s">
         <v>358</v>
       </c>
       <c r="M55" t="s">
         <v>162</v>
+      </c>
+      <c r="N55" s="2">
+        <v>1</v>
       </c>
       <c r="O55" t="s">
         <v>208</v>
@@ -3238,13 +3305,20 @@
         <f>E14</f>
         <v>12</v>
       </c>
-      <c r="C56" s="11">
+      <c r="C56" s="12">
         <f>F14</f>
         <v>12</v>
       </c>
+      <c r="D56" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="E56" t="s">
         <v>177</v>
       </c>
+      <c r="F56" s="2">
+        <v>1</v>
+      </c>
       <c r="I56" t="s">
         <v>357</v>
       </c>
@@ -3253,7 +3327,7 @@
       </c>
       <c r="N56" s="2">
         <f>SUM(N49:N55)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O56" t="s">
         <v>210</v>
@@ -3273,12 +3347,19 @@
         <f>G14</f>
         <v>12</v>
       </c>
-      <c r="C57" s="11">
+      <c r="C57" s="12">
         <f>H14</f>
         <v>12</v>
       </c>
+      <c r="D57" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="E57" t="s">
         <v>176</v>
+      </c>
+      <c r="F57" s="2">
+        <v>1</v>
       </c>
       <c r="I57" t="s">
         <v>345</v>
@@ -3301,12 +3382,19 @@
         <f>I4</f>
         <v>2</v>
       </c>
-      <c r="C58" s="11">
+      <c r="C58" s="12">
         <f>J4</f>
         <v>0</v>
       </c>
+      <c r="D58" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E58" t="s">
         <v>179</v>
+      </c>
+      <c r="F58" s="2">
+        <v>1</v>
       </c>
       <c r="I58" t="s">
         <v>119</v>
@@ -3329,12 +3417,19 @@
         <f>K10</f>
         <v>8</v>
       </c>
-      <c r="C59" s="11">
+      <c r="C59" s="12">
         <f>L10</f>
         <v>0</v>
       </c>
+      <c r="D59" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E59" t="s">
         <v>189</v>
+      </c>
+      <c r="F59" s="2">
+        <v>1</v>
       </c>
       <c r="I59" t="s">
         <v>120</v>
@@ -3357,12 +3452,19 @@
         <f>M31</f>
         <v>29</v>
       </c>
-      <c r="C60" s="11">
+      <c r="C60" s="12">
         <f>N31</f>
         <v>0</v>
       </c>
+      <c r="D60" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E60" t="s">
         <v>175</v>
+      </c>
+      <c r="F60" s="2">
+        <v>1</v>
       </c>
       <c r="I60" t="s">
         <v>346</v>
@@ -3385,12 +3487,19 @@
         <f>O99</f>
         <v>97</v>
       </c>
-      <c r="C61" s="11">
+      <c r="C61" s="12">
         <f>P99</f>
         <v>56</v>
       </c>
+      <c r="D61" s="16">
+        <f t="shared" si="0"/>
+        <v>0.57731958762886593</v>
+      </c>
       <c r="E61" t="s">
         <v>173</v>
+      </c>
+      <c r="F61" s="2">
+        <v>1</v>
       </c>
       <c r="I61" t="s">
         <v>361</v>
@@ -3414,12 +3523,19 @@
         <f>Q8</f>
         <v>6</v>
       </c>
-      <c r="C62" s="11">
+      <c r="C62" s="12">
         <f>R8</f>
         <v>0</v>
       </c>
+      <c r="D62" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E62" t="s">
         <v>172</v>
+      </c>
+      <c r="F62" s="2">
+        <v>1</v>
       </c>
       <c r="I62" t="s">
         <v>362</v>
@@ -3436,12 +3552,19 @@
         <f>E38</f>
         <v>7</v>
       </c>
-      <c r="C63" s="11">
+      <c r="C63" s="12">
         <f>F38</f>
         <v>0</v>
       </c>
+      <c r="D63" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E63" t="s">
         <v>171</v>
+      </c>
+      <c r="F63" s="2">
+        <v>1</v>
       </c>
       <c r="I63" t="s">
         <v>352</v>
@@ -3458,12 +3581,19 @@
         <f>G35</f>
         <v>4</v>
       </c>
-      <c r="C64" s="11">
+      <c r="C64" s="12">
         <f>H35</f>
         <v>0</v>
       </c>
+      <c r="D64" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E64" t="s">
         <v>174</v>
+      </c>
+      <c r="F64" s="2">
+        <v>1</v>
       </c>
       <c r="I64" t="s">
         <v>353</v>
@@ -3483,12 +3613,19 @@
         <f>I33</f>
         <v>2</v>
       </c>
-      <c r="C65" s="11">
+      <c r="C65" s="12">
         <f>J33</f>
         <v>2</v>
       </c>
+      <c r="D65" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="E65" t="s">
         <v>181</v>
+      </c>
+      <c r="F65" s="2">
+        <v>1</v>
       </c>
       <c r="I65" t="s">
         <v>369</v>
@@ -3508,12 +3645,19 @@
         <f>K33</f>
         <v>2</v>
       </c>
-      <c r="C66" s="11">
+      <c r="C66" s="12">
         <f>L33</f>
         <v>0</v>
       </c>
+      <c r="D66" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E66" t="s">
         <v>183</v>
+      </c>
+      <c r="F66" s="2">
+        <v>1</v>
       </c>
       <c r="I66" t="s">
         <v>336</v>
@@ -3530,12 +3674,19 @@
         <f>M41</f>
         <v>8</v>
       </c>
-      <c r="C67" s="11">
+      <c r="C67" s="12">
         <f>N41</f>
         <v>0</v>
       </c>
+      <c r="D67" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E67" t="s">
         <v>182</v>
+      </c>
+      <c r="F67" s="2">
+        <v>1</v>
       </c>
       <c r="I67" t="s">
         <v>118</v>
@@ -3552,16 +3703,20 @@
         <f>Q61</f>
         <v>29</v>
       </c>
-      <c r="C68" s="11">
+      <c r="C68" s="12">
         <f>R61</f>
         <v>0</v>
       </c>
+      <c r="D68" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E68" s="4">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F68" s="2">
         <f>SUM(F49:F67)</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="I68" t="s">
         <v>341</v>
@@ -3579,11 +3734,15 @@
       </c>
       <c r="B69" s="9">
         <f>E68</f>
-        <v>20</v>
-      </c>
-      <c r="C69" s="11">
+        <v>19</v>
+      </c>
+      <c r="C69" s="12">
         <f>F68</f>
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="D69" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="I69" t="s">
         <v>342</v>
@@ -3603,9 +3762,13 @@
         <f>G52</f>
         <v>3</v>
       </c>
-      <c r="C70" s="11">
+      <c r="C70" s="12">
         <f>H52</f>
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D70" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="I70" t="s">
         <v>340</v>
@@ -3625,8 +3788,12 @@
         <f>I91</f>
         <v>42</v>
       </c>
-      <c r="C71" s="11">
+      <c r="C71" s="12">
         <f>J91</f>
+        <v>0</v>
+      </c>
+      <c r="D71" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I71" t="s">
@@ -3647,9 +3814,13 @@
         <f>K50</f>
         <v>1</v>
       </c>
-      <c r="C72" s="11">
+      <c r="C72" s="12">
         <f>L50</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D72" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="I72" t="s">
         <v>344</v>
@@ -3669,9 +3840,13 @@
         <f>M56</f>
         <v>7</v>
       </c>
-      <c r="C73" s="11">
+      <c r="C73" s="12">
         <f>N56</f>
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="D73" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="I73" t="s">
         <v>351</v>
@@ -3683,7 +3858,8 @@
     <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" s="10"/>
       <c r="B74" s="9"/>
-      <c r="C74" s="11"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="9"/>
       <c r="I74" t="s">
         <v>347</v>
       </c>
@@ -3695,12 +3871,13 @@
       <c r="A75" s="10"/>
       <c r="B75" s="9">
         <f>SUM(B54:B74)</f>
-        <v>377</v>
-      </c>
-      <c r="C75" s="11">
+        <v>376</v>
+      </c>
+      <c r="C75" s="12">
         <f>SUM(C54:C74)</f>
-        <v>142</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="D75" s="9"/>
       <c r="I75" t="s">
         <v>348</v>
       </c>
@@ -3709,12 +3886,13 @@
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A76" s="12"/>
-      <c r="B76" s="13">
+      <c r="A76" s="13"/>
+      <c r="B76" s="14">
         <f>C75/B75</f>
-        <v>0.37665782493368699</v>
-      </c>
-      <c r="C76" s="12"/>
+        <v>0.45744680851063829</v>
+      </c>
+      <c r="C76" s="13"/>
+      <c r="D76" s="9"/>
       <c r="I76" t="s">
         <v>349</v>
       </c>

</xml_diff>

<commit_message>
README & NuGet Version Bump
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\coding\dotPDFium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9684D9E2-44E7-4360-B22A-07EDD6FCD8FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4AEF3C-2D08-4BFD-8E7E-5D454E6835D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39090" yWindow="870" windowWidth="36190" windowHeight="19510" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
+    <workbookView xWindow="740" yWindow="910" windowWidth="36190" windowHeight="19510" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1699,7 +1699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93991F7-7A9D-4291-8EC0-AB472EBDEDBD}">
   <dimension ref="A1:R99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
Font glyphs & Textual cross-index lookup.
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\coding\dotPDFium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4AEF3C-2D08-4BFD-8E7E-5D454E6835D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B04AC2-4C76-45FC-9F13-E93D1C31997F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="910" windowWidth="36190" windowHeight="19510" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
+    <workbookView xWindow="39110" yWindow="810" windowWidth="36190" windowHeight="19510" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="397">
   <si>
     <t>Text_LoadPage</t>
   </si>
@@ -996,9 +996,6 @@
   </si>
   <si>
     <t>PdfDataAvailNative</t>
-  </si>
-  <si>
-    <t>PefEditNative</t>
   </si>
   <si>
     <t>PdfExtNative</t>
@@ -1699,7 +1696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93991F7-7A9D-4291-8EC0-AB472EBDEDBD}">
   <dimension ref="A1:R99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1746,15 +1743,15 @@
         <v>318</v>
       </c>
       <c r="O1" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>320</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -1807,7 +1804,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H3" s="2">
         <v>1</v>
@@ -1907,6 +1904,9 @@
       <c r="O5" t="s">
         <v>232</v>
       </c>
+      <c r="P5" s="2">
+        <v>1</v>
+      </c>
       <c r="Q5" t="s">
         <v>110</v>
       </c>
@@ -1942,6 +1942,9 @@
       <c r="O6" t="s">
         <v>225</v>
       </c>
+      <c r="P6" s="2">
+        <v>1</v>
+      </c>
       <c r="Q6" t="s">
         <v>109</v>
       </c>
@@ -1977,6 +1980,9 @@
       <c r="O7" t="s">
         <v>233</v>
       </c>
+      <c r="P7" s="2">
+        <v>1</v>
+      </c>
       <c r="Q7" t="s">
         <v>113</v>
       </c>
@@ -2012,6 +2018,9 @@
       <c r="O8" t="s">
         <v>226</v>
       </c>
+      <c r="P8" s="2">
+        <v>1</v>
+      </c>
       <c r="Q8" s="4">
         <v>6</v>
       </c>
@@ -2054,6 +2063,9 @@
       <c r="O9" t="s">
         <v>229</v>
       </c>
+      <c r="P9" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -2093,6 +2105,9 @@
       <c r="O10" t="s">
         <v>227</v>
       </c>
+      <c r="P10" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -2125,6 +2140,9 @@
       <c r="O11" t="s">
         <v>235</v>
       </c>
+      <c r="P11" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -2157,6 +2175,9 @@
       <c r="O12" t="s">
         <v>234</v>
       </c>
+      <c r="P12" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -2186,6 +2207,9 @@
       <c r="O13" t="s">
         <v>228</v>
       </c>
+      <c r="P13" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -2220,6 +2244,9 @@
       <c r="O14" t="s">
         <v>231</v>
       </c>
+      <c r="P14" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -2240,6 +2267,9 @@
       <c r="O15" t="s">
         <v>230</v>
       </c>
+      <c r="P15" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -2252,7 +2282,7 @@
         <v>293</v>
       </c>
       <c r="M16" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="O16" t="s">
         <v>238</v>
@@ -2269,7 +2299,7 @@
         <v>295</v>
       </c>
       <c r="M17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="O17" t="s">
         <v>239</v>
@@ -2286,10 +2316,13 @@
         <v>292</v>
       </c>
       <c r="M18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="O18" t="s">
         <v>236</v>
+      </c>
+      <c r="P18" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.35">
@@ -2306,10 +2339,13 @@
         <v>1</v>
       </c>
       <c r="M19" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="O19" t="s">
         <v>237</v>
+      </c>
+      <c r="P19" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
@@ -2323,7 +2359,7 @@
         <v>309</v>
       </c>
       <c r="M20" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="O20" t="s">
         <v>261</v>
@@ -2343,7 +2379,7 @@
         <v>308</v>
       </c>
       <c r="M21" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="O21" t="s">
         <v>255</v>
@@ -2366,7 +2402,7 @@
         <v>1</v>
       </c>
       <c r="M22" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O22" t="s">
         <v>256</v>
@@ -2389,7 +2425,7 @@
         <v>1</v>
       </c>
       <c r="M23" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="O23" t="s">
         <v>258</v>
@@ -2435,7 +2471,7 @@
         <v>1</v>
       </c>
       <c r="M25" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="O25" t="s">
         <v>259</v>
@@ -2458,7 +2494,7 @@
         <v>1</v>
       </c>
       <c r="M26" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="O26" t="s">
         <v>260</v>
@@ -2557,19 +2593,19 @@
         <v>296</v>
       </c>
       <c r="E30" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="G30" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="I30" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="I30" s="6" t="s">
+      <c r="K30" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="K30" s="6" t="s">
-        <v>373</v>
-      </c>
       <c r="M30" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O30" t="s">
         <v>100</v>
@@ -2578,7 +2614,7 @@
         <v>1</v>
       </c>
       <c r="Q30" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2606,6 +2642,9 @@
       <c r="K31" t="s">
         <v>137</v>
       </c>
+      <c r="L31" s="2">
+        <v>1</v>
+      </c>
       <c r="M31" s="8">
         <v>29</v>
       </c>
@@ -2620,7 +2659,7 @@
         <v>1</v>
       </c>
       <c r="Q31" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.35">
@@ -2648,8 +2687,11 @@
       <c r="K32" t="s">
         <v>138</v>
       </c>
+      <c r="L32" s="2">
+        <v>1</v>
+      </c>
       <c r="M32" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="O32" t="s">
         <v>193</v>
@@ -2658,7 +2700,7 @@
         <v>1</v>
       </c>
       <c r="Q32" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
@@ -2689,7 +2731,7 @@
       </c>
       <c r="L33" s="2">
         <f>SUM(L31:L32)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M33" t="s">
         <v>139</v>
@@ -2701,7 +2743,7 @@
         <v>1</v>
       </c>
       <c r="Q33" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
@@ -2730,7 +2772,7 @@
         <v>1</v>
       </c>
       <c r="Q34" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.35">
@@ -2766,7 +2808,7 @@
         <v>1</v>
       </c>
       <c r="Q35" s="7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
@@ -2795,7 +2837,7 @@
         <v>1</v>
       </c>
       <c r="Q36" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
@@ -2820,8 +2862,11 @@
       <c r="O37" t="s">
         <v>198</v>
       </c>
+      <c r="P37" s="2">
+        <v>1</v>
+      </c>
       <c r="Q37" s="7" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
@@ -2852,7 +2897,7 @@
         <v>242</v>
       </c>
       <c r="Q38" s="7" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
@@ -2869,7 +2914,7 @@
         <v>240</v>
       </c>
       <c r="Q39" s="7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
@@ -2889,7 +2934,7 @@
         <v>1</v>
       </c>
       <c r="Q40" s="7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
@@ -2961,7 +3006,7 @@
         <v>1</v>
       </c>
       <c r="Q44" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.35">
@@ -2972,7 +3017,7 @@
         <v>265</v>
       </c>
       <c r="Q45" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.35">
@@ -3005,7 +3050,7 @@
         <v>262</v>
       </c>
       <c r="Q47" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.35">
@@ -3013,19 +3058,19 @@
         <v>303</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="O48" t="s">
         <v>206</v>
@@ -3150,7 +3195,7 @@
         <v>269</v>
       </c>
       <c r="Q51" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.35">
@@ -3185,7 +3230,7 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A53" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
@@ -3238,10 +3283,10 @@
         <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="M54" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="N54" s="2">
         <v>1</v>
@@ -3253,7 +3298,7 @@
         <v>1</v>
       </c>
       <c r="Q54" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.35">
@@ -3279,7 +3324,7 @@
         <v>1</v>
       </c>
       <c r="I55" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M55" t="s">
         <v>162</v>
@@ -3320,7 +3365,7 @@
         <v>1</v>
       </c>
       <c r="I56" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="M56" s="4">
         <v>7</v>
@@ -3362,7 +3407,7 @@
         <v>1</v>
       </c>
       <c r="I57" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="O57" t="s">
         <v>191</v>
@@ -3467,7 +3512,7 @@
         <v>1</v>
       </c>
       <c r="I60" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="O60" t="s">
         <v>104</v>
@@ -3481,7 +3526,7 @@
     </row>
     <row r="61" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B61" s="9">
         <f>O99</f>
@@ -3489,11 +3534,11 @@
       </c>
       <c r="C61" s="12">
         <f>P99</f>
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="D61" s="16">
         <f t="shared" si="0"/>
-        <v>0.57731958762886593</v>
+        <v>0.72164948453608246</v>
       </c>
       <c r="E61" t="s">
         <v>173</v>
@@ -3502,7 +3547,7 @@
         <v>1</v>
       </c>
       <c r="I61" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="O61" t="s">
         <v>243</v>
@@ -3517,7 +3562,7 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A62" s="10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B62" s="9">
         <f>Q8</f>
@@ -3538,7 +3583,7 @@
         <v>1</v>
       </c>
       <c r="I62" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="O62" t="s">
         <v>266</v>
@@ -3546,7 +3591,7 @@
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A63" s="10" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B63" s="9">
         <f>E38</f>
@@ -3567,7 +3612,7 @@
         <v>1</v>
       </c>
       <c r="I63" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="O63" t="s">
         <v>263</v>
@@ -3575,7 +3620,7 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A64" s="10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B64" s="9">
         <f>G35</f>
@@ -3596,7 +3641,7 @@
         <v>1</v>
       </c>
       <c r="I64" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="O64" t="s">
         <v>205</v>
@@ -3607,7 +3652,7 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B65" s="9">
         <f>I33</f>
@@ -3628,7 +3673,7 @@
         <v>1</v>
       </c>
       <c r="I65" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="O65" t="s">
         <v>195</v>
@@ -3639,7 +3684,7 @@
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="10" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B66" s="9">
         <f>K33</f>
@@ -3647,11 +3692,11 @@
       </c>
       <c r="C66" s="12">
         <f>L33</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D66" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E66" t="s">
         <v>183</v>
@@ -3660,7 +3705,7 @@
         <v>1</v>
       </c>
       <c r="I66" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="O66" t="s">
         <v>272</v>
@@ -3668,7 +3713,7 @@
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B67" s="9">
         <f>M41</f>
@@ -3697,7 +3742,7 @@
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B68" s="9">
         <f>Q61</f>
@@ -3719,7 +3764,7 @@
         <v>19</v>
       </c>
       <c r="I68" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="O68" t="s">
         <v>197</v>
@@ -3730,7 +3775,7 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B69" s="9">
         <f>E68</f>
@@ -3745,7 +3790,7 @@
         <v>1</v>
       </c>
       <c r="I69" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="O69" t="s">
         <v>207</v>
@@ -3756,7 +3801,7 @@
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B70" s="9">
         <f>G52</f>
@@ -3771,7 +3816,7 @@
         <v>1</v>
       </c>
       <c r="I70" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="O70" t="s">
         <v>209</v>
@@ -3782,7 +3827,7 @@
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B71" s="9">
         <f>I91</f>
@@ -3797,7 +3842,7 @@
         <v>0</v>
       </c>
       <c r="I71" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="O71" t="s">
         <v>102</v>
@@ -3808,7 +3853,7 @@
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B72" s="9">
         <f>K50</f>
@@ -3823,7 +3868,7 @@
         <v>1</v>
       </c>
       <c r="I72" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="O72" t="s">
         <v>204</v>
@@ -3834,7 +3879,7 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B73" s="9">
         <f>M56</f>
@@ -3849,7 +3894,7 @@
         <v>1</v>
       </c>
       <c r="I73" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="O73" t="s">
         <v>245</v>
@@ -3861,7 +3906,7 @@
       <c r="C74" s="12"/>
       <c r="D74" s="9"/>
       <c r="I74" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="O74" t="s">
         <v>244</v>
@@ -3875,11 +3920,11 @@
       </c>
       <c r="C75" s="12">
         <f>SUM(C54:C74)</f>
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="D75" s="9"/>
       <c r="I75" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="O75" t="s">
         <v>250</v>
@@ -3889,12 +3934,12 @@
       <c r="A76" s="13"/>
       <c r="B76" s="14">
         <f>C75/B75</f>
-        <v>0.45744680851063829</v>
+        <v>0.5</v>
       </c>
       <c r="C76" s="13"/>
       <c r="D76" s="9"/>
       <c r="I76" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="O76" t="s">
         <v>248</v>
@@ -3902,7 +3947,7 @@
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="I77" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="O77" t="s">
         <v>246</v>
@@ -3910,7 +3955,7 @@
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="I78" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="O78" t="s">
         <v>249</v>
@@ -3918,7 +3963,7 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="I79" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="O79" t="s">
         <v>247</v>
@@ -3926,7 +3971,7 @@
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="I80" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="O80" t="s">
         <v>254</v>
@@ -3934,7 +3979,7 @@
     </row>
     <row r="81" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I81" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="O81" t="s">
         <v>253</v>
@@ -3942,7 +3987,7 @@
     </row>
     <row r="82" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I82" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="O82" t="s">
         <v>251</v>
@@ -3950,7 +3995,7 @@
     </row>
     <row r="83" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I83" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="O83" t="s">
         <v>252</v>
@@ -3958,7 +4003,7 @@
     </row>
     <row r="84" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I84" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O84" t="s">
         <v>215</v>
@@ -3969,7 +4014,7 @@
     </row>
     <row r="85" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I85" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="O85" t="s">
         <v>217</v>
@@ -3980,7 +4025,7 @@
     </row>
     <row r="86" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I86" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="O86" t="s">
         <v>214</v>
@@ -3991,7 +4036,7 @@
     </row>
     <row r="87" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I87" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="O87" t="s">
         <v>213</v>
@@ -4002,7 +4047,7 @@
     </row>
     <row r="88" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I88" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="O88" t="s">
         <v>216</v>
@@ -4013,7 +4058,7 @@
     </row>
     <row r="89" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I89" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="O89" t="s">
         <v>218</v>
@@ -4024,7 +4069,7 @@
     </row>
     <row r="90" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I90" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="O90" t="s">
         <v>192</v>
@@ -4110,7 +4155,7 @@
       </c>
       <c r="P99" s="2">
         <f>SUM(P2:P98)</f>
-        <v>56</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work on marks, actions, web links, document links & destinations.
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\coding\dotPDFium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B04AC2-4C76-45FC-9F13-E93D1C31997F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD644B3C-AD4F-4189-BB7B-6FF13B888CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39110" yWindow="810" windowWidth="36190" windowHeight="19510" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="398">
   <si>
     <t>Text_LoadPage</t>
   </si>
@@ -1227,6 +1227,9 @@
   </si>
   <si>
     <t>Link_CloseWebLinks</t>
+  </si>
+  <si>
+    <t>Dest_GetPageIndex</t>
   </si>
 </sst>
 </file>
@@ -1753,6 +1756,9 @@
       <c r="A2" t="s">
         <v>396</v>
       </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
       <c r="C2" t="s">
         <v>29</v>
       </c>
@@ -1783,14 +1789,23 @@
       <c r="O2" t="s">
         <v>268</v>
       </c>
+      <c r="P2" s="2">
+        <v>1</v>
+      </c>
       <c r="Q2" t="s">
         <v>112</v>
+      </c>
+      <c r="R2" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>288</v>
       </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
       <c r="C3" t="s">
         <v>30</v>
       </c>
@@ -1826,12 +1841,18 @@
       </c>
       <c r="Q3" t="s">
         <v>114</v>
+      </c>
+      <c r="R3" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>286</v>
       </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
       <c r="C4" t="s">
         <v>31</v>
       </c>
@@ -1863,6 +1884,9 @@
       <c r="M4" t="s">
         <v>84</v>
       </c>
+      <c r="N4" s="2">
+        <v>1</v>
+      </c>
       <c r="O4" t="s">
         <v>108</v>
       </c>
@@ -1871,12 +1895,18 @@
       </c>
       <c r="Q4" t="s">
         <v>111</v>
+      </c>
+      <c r="R4" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>289</v>
       </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
       <c r="C5" t="s">
         <v>37</v>
       </c>
@@ -1901,6 +1931,9 @@
       <c r="M5" t="s">
         <v>85</v>
       </c>
+      <c r="N5" s="2">
+        <v>1</v>
+      </c>
       <c r="O5" t="s">
         <v>232</v>
       </c>
@@ -1909,12 +1942,18 @@
       </c>
       <c r="Q5" t="s">
         <v>110</v>
+      </c>
+      <c r="R5" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>290</v>
       </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
       <c r="C6" t="s">
         <v>32</v>
       </c>
@@ -1939,6 +1978,9 @@
       <c r="M6" t="s">
         <v>83</v>
       </c>
+      <c r="N6" s="2">
+        <v>1</v>
+      </c>
       <c r="O6" t="s">
         <v>225</v>
       </c>
@@ -1947,12 +1989,18 @@
       </c>
       <c r="Q6" t="s">
         <v>109</v>
+      </c>
+      <c r="R6" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>287</v>
       </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
       <c r="C7" t="s">
         <v>36</v>
       </c>
@@ -1977,6 +2025,9 @@
       <c r="M7" t="s">
         <v>86</v>
       </c>
+      <c r="N7" s="2">
+        <v>1</v>
+      </c>
       <c r="O7" t="s">
         <v>233</v>
       </c>
@@ -1985,12 +2036,18 @@
       </c>
       <c r="Q7" t="s">
         <v>113</v>
+      </c>
+      <c r="R7" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>285</v>
       </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
       <c r="C8" t="s">
         <v>34</v>
       </c>
@@ -2026,7 +2083,7 @@
       </c>
       <c r="R8" s="2">
         <f>SUM(R2:R7)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
@@ -2299,7 +2356,7 @@
         <v>295</v>
       </c>
       <c r="M17" t="s">
-        <v>327</v>
+        <v>397</v>
       </c>
       <c r="O17" t="s">
         <v>239</v>
@@ -2316,7 +2373,7 @@
         <v>292</v>
       </c>
       <c r="M18" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="O18" t="s">
         <v>236</v>
@@ -2339,7 +2396,7 @@
         <v>1</v>
       </c>
       <c r="M19" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="O19" t="s">
         <v>237</v>
@@ -2359,7 +2416,7 @@
         <v>309</v>
       </c>
       <c r="M20" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="O20" t="s">
         <v>261</v>
@@ -2379,7 +2436,7 @@
         <v>308</v>
       </c>
       <c r="M21" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="O21" t="s">
         <v>255</v>
@@ -2402,7 +2459,7 @@
         <v>1</v>
       </c>
       <c r="M22" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="O22" t="s">
         <v>256</v>
@@ -2425,7 +2482,10 @@
         <v>1</v>
       </c>
       <c r="M23" t="s">
-        <v>322</v>
+        <v>325</v>
+      </c>
+      <c r="N23" s="2">
+        <v>1</v>
       </c>
       <c r="O23" t="s">
         <v>258</v>
@@ -2448,7 +2508,10 @@
         <v>1</v>
       </c>
       <c r="M24" t="s">
-        <v>93</v>
+        <v>322</v>
+      </c>
+      <c r="N24" s="2">
+        <v>1</v>
       </c>
       <c r="O24" t="s">
         <v>257</v>
@@ -2471,7 +2534,10 @@
         <v>1</v>
       </c>
       <c r="M25" t="s">
-        <v>323</v>
+        <v>93</v>
+      </c>
+      <c r="N25" s="2">
+        <v>1</v>
       </c>
       <c r="O25" t="s">
         <v>259</v>
@@ -2494,7 +2560,10 @@
         <v>1</v>
       </c>
       <c r="M26" t="s">
-        <v>324</v>
+        <v>323</v>
+      </c>
+      <c r="N26" s="2">
+        <v>0</v>
       </c>
       <c r="O26" t="s">
         <v>260</v>
@@ -2517,7 +2586,10 @@
         <v>1</v>
       </c>
       <c r="M27" t="s">
-        <v>92</v>
+        <v>324</v>
+      </c>
+      <c r="N27" s="2">
+        <v>1</v>
       </c>
       <c r="O27" t="s">
         <v>99</v>
@@ -2540,7 +2612,10 @@
         <v>1</v>
       </c>
       <c r="M28" t="s">
-        <v>90</v>
+        <v>92</v>
+      </c>
+      <c r="N28" s="2">
+        <v>1</v>
       </c>
       <c r="O28" t="s">
         <v>96</v>
@@ -2571,7 +2646,10 @@
       <c r="K29" s="1"/>
       <c r="L29" s="3"/>
       <c r="M29" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="N29" s="2">
+        <v>1</v>
       </c>
       <c r="O29" t="s">
         <v>98</v>
@@ -2605,7 +2683,10 @@
         <v>372</v>
       </c>
       <c r="M30" t="s">
-        <v>326</v>
+        <v>91</v>
+      </c>
+      <c r="N30" s="2">
+        <v>1</v>
       </c>
       <c r="O30" t="s">
         <v>100</v>
@@ -2617,7 +2698,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -2645,12 +2726,11 @@
       <c r="L31" s="2">
         <v>1</v>
       </c>
-      <c r="M31" s="8">
-        <v>29</v>
-      </c>
-      <c r="N31" s="3">
-        <f>SUM(N2:N30)</f>
-        <v>0</v>
+      <c r="M31" t="s">
+        <v>326</v>
+      </c>
+      <c r="N31" s="2">
+        <v>1</v>
       </c>
       <c r="O31" t="s">
         <v>200</v>
@@ -2662,7 +2742,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>273</v>
       </c>
@@ -2690,8 +2770,12 @@
       <c r="L32" s="2">
         <v>1</v>
       </c>
-      <c r="M32" s="6" t="s">
-        <v>373</v>
+      <c r="M32" s="8">
+        <v>30</v>
+      </c>
+      <c r="N32" s="3">
+        <f>SUM(N2:N31)</f>
+        <v>12</v>
       </c>
       <c r="O32" t="s">
         <v>193</v>
@@ -2733,8 +2817,8 @@
         <f>SUM(L31:L32)</f>
         <v>2</v>
       </c>
-      <c r="M33" t="s">
-        <v>139</v>
+      <c r="M33" s="6" t="s">
+        <v>373</v>
       </c>
       <c r="O33" t="s">
         <v>97</v>
@@ -2763,7 +2847,7 @@
         <v>132</v>
       </c>
       <c r="M34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O34" t="s">
         <v>95</v>
@@ -2799,7 +2883,7 @@
         <v>0</v>
       </c>
       <c r="M35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="O35" t="s">
         <v>202</v>
@@ -2828,7 +2912,7 @@
         <v>129</v>
       </c>
       <c r="M36" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="O36" t="s">
         <v>201</v>
@@ -2857,7 +2941,7 @@
         <v>127</v>
       </c>
       <c r="M37" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="O37" t="s">
         <v>198</v>
@@ -2875,7 +2959,7 @@
       </c>
       <c r="B38" s="2">
         <f>SUM(B2:B37)</f>
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C38" t="s">
         <v>19</v>
@@ -2891,10 +2975,13 @@
         <v>0</v>
       </c>
       <c r="M38" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="O38" t="s">
         <v>242</v>
+      </c>
+      <c r="P38" s="2">
+        <v>1</v>
       </c>
       <c r="Q38" s="7" t="s">
         <v>383</v>
@@ -2908,10 +2995,13 @@
         <v>1</v>
       </c>
       <c r="M39" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="O39" t="s">
         <v>240</v>
+      </c>
+      <c r="P39" s="2">
+        <v>1</v>
       </c>
       <c r="Q39" s="7" t="s">
         <v>380</v>
@@ -2925,7 +3015,7 @@
         <v>1</v>
       </c>
       <c r="M40" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="O40" t="s">
         <v>211</v>
@@ -2944,12 +3034,8 @@
       <c r="D41" s="2">
         <v>1</v>
       </c>
-      <c r="M41" s="4">
-        <v>8</v>
-      </c>
-      <c r="N41" s="2">
-        <f>SUM(N33:N40)</f>
-        <v>0</v>
+      <c r="M41" t="s">
+        <v>145</v>
       </c>
       <c r="O41" t="s">
         <v>212</v>
@@ -2967,6 +3053,13 @@
       </c>
       <c r="D42" s="2">
         <v>1</v>
+      </c>
+      <c r="M42" s="4">
+        <v>8</v>
+      </c>
+      <c r="N42" s="2">
+        <f>SUM(N34:N41)</f>
+        <v>0</v>
       </c>
       <c r="O42" t="s">
         <v>107</v>
@@ -3045,7 +3138,6 @@
       <c r="J47" s="3"/>
       <c r="K47" s="1"/>
       <c r="L47" s="3"/>
-      <c r="M47" s="1"/>
       <c r="O47" t="s">
         <v>262</v>
       </c>
@@ -3053,7 +3145,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C48" t="s">
         <v>303</v>
       </c>
@@ -3069,9 +3161,7 @@
       <c r="K48" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="M48" s="5" t="s">
-        <v>390</v>
-      </c>
+      <c r="M48" s="1"/>
       <c r="O48" t="s">
         <v>206</v>
       </c>
@@ -3107,11 +3197,8 @@
       <c r="L49" s="2">
         <v>1</v>
       </c>
-      <c r="M49" t="s">
-        <v>165</v>
-      </c>
-      <c r="N49" s="2">
-        <v>1</v>
+      <c r="M49" s="5" t="s">
+        <v>390</v>
       </c>
       <c r="O49" t="s">
         <v>194</v>
@@ -3150,7 +3237,7 @@
         <v>1</v>
       </c>
       <c r="M50" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="N50" s="2">
         <v>1</v>
@@ -3186,7 +3273,7 @@
         <v>123</v>
       </c>
       <c r="M51" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="N51" s="2">
         <v>1</v>
@@ -3216,13 +3303,16 @@
         <v>117</v>
       </c>
       <c r="M52" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="N52" s="2">
         <v>1</v>
       </c>
       <c r="O52" t="s">
         <v>241</v>
+      </c>
+      <c r="P52" s="2">
+        <v>1</v>
       </c>
       <c r="Q52" t="s">
         <v>160</v>
@@ -3245,7 +3335,7 @@
         <v>116</v>
       </c>
       <c r="M53" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N53" s="2">
         <v>1</v>
@@ -3270,11 +3360,11 @@
       </c>
       <c r="C54" s="12">
         <f>B38</f>
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D54" s="16">
         <f>C54/B54</f>
-        <v>0.80555555555555558</v>
+        <v>1</v>
       </c>
       <c r="E54" t="s">
         <v>180</v>
@@ -3286,7 +3376,7 @@
         <v>336</v>
       </c>
       <c r="M54" t="s">
-        <v>391</v>
+        <v>167</v>
       </c>
       <c r="N54" s="2">
         <v>1</v>
@@ -3327,7 +3417,7 @@
         <v>357</v>
       </c>
       <c r="M55" t="s">
-        <v>162</v>
+        <v>391</v>
       </c>
       <c r="N55" s="2">
         <v>1</v>
@@ -3367,12 +3457,11 @@
       <c r="I56" t="s">
         <v>356</v>
       </c>
-      <c r="M56" s="4">
-        <v>7</v>
+      <c r="M56" t="s">
+        <v>162</v>
       </c>
       <c r="N56" s="2">
-        <f>SUM(N49:N55)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="O56" t="s">
         <v>210</v>
@@ -3409,6 +3498,13 @@
       <c r="I57" t="s">
         <v>344</v>
       </c>
+      <c r="M57" s="4">
+        <v>7</v>
+      </c>
+      <c r="N57" s="2">
+        <f>SUM(N50:N56)</f>
+        <v>7</v>
+      </c>
       <c r="O57" t="s">
         <v>191</v>
       </c>
@@ -3494,16 +3590,16 @@
         <v>318</v>
       </c>
       <c r="B60" s="9">
-        <f>M31</f>
-        <v>29</v>
+        <f>M32</f>
+        <v>30</v>
       </c>
       <c r="C60" s="12">
-        <f>N31</f>
-        <v>0</v>
+        <f>N32</f>
+        <v>12</v>
       </c>
       <c r="D60" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E60" t="s">
         <v>175</v>
@@ -3534,11 +3630,11 @@
       </c>
       <c r="C61" s="12">
         <f>P99</f>
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="D61" s="16">
         <f t="shared" si="0"/>
-        <v>0.72164948453608246</v>
+        <v>0.88659793814432986</v>
       </c>
       <c r="E61" t="s">
         <v>173</v>
@@ -3551,6 +3647,9 @@
       </c>
       <c r="O61" t="s">
         <v>243</v>
+      </c>
+      <c r="P61" s="2">
+        <v>1</v>
       </c>
       <c r="Q61" s="8">
         <v>29</v>
@@ -3570,11 +3669,11 @@
       </c>
       <c r="C62" s="12">
         <f>R8</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D62" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62" t="s">
         <v>172</v>
@@ -3716,11 +3815,11 @@
         <v>373</v>
       </c>
       <c r="B67" s="9">
-        <f>M41</f>
+        <f>M42</f>
         <v>8</v>
       </c>
       <c r="C67" s="12">
-        <f>N41</f>
+        <f>N42</f>
         <v>0</v>
       </c>
       <c r="D67" s="16">
@@ -3882,11 +3981,11 @@
         <v>390</v>
       </c>
       <c r="B73" s="9">
-        <f>M56</f>
+        <f>M57</f>
         <v>7</v>
       </c>
       <c r="C73" s="12">
-        <f>N56</f>
+        <f>N57</f>
         <v>7</v>
       </c>
       <c r="D73" s="16">
@@ -3898,6 +3997,9 @@
       </c>
       <c r="O73" t="s">
         <v>245</v>
+      </c>
+      <c r="P73" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.35">
@@ -3911,16 +4013,19 @@
       <c r="O74" t="s">
         <v>244</v>
       </c>
+      <c r="P74" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" s="10"/>
       <c r="B75" s="9">
         <f>SUM(B54:B74)</f>
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C75" s="12">
         <f>SUM(C54:C74)</f>
-        <v>188</v>
+        <v>229</v>
       </c>
       <c r="D75" s="9"/>
       <c r="I75" t="s">
@@ -3928,13 +4033,16 @@
       </c>
       <c r="O75" t="s">
         <v>250</v>
+      </c>
+      <c r="P75" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" s="13"/>
       <c r="B76" s="14">
         <f>C75/B75</f>
-        <v>0.5</v>
+        <v>0.60742705570291777</v>
       </c>
       <c r="C76" s="13"/>
       <c r="D76" s="9"/>
@@ -3944,6 +4052,9 @@
       <c r="O76" t="s">
         <v>248</v>
       </c>
+      <c r="P76" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="I77" t="s">
@@ -3952,6 +4063,9 @@
       <c r="O77" t="s">
         <v>246</v>
       </c>
+      <c r="P77" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="I78" t="s">
@@ -3960,6 +4074,9 @@
       <c r="O78" t="s">
         <v>249</v>
       </c>
+      <c r="P78" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="I79" t="s">
@@ -3968,6 +4085,9 @@
       <c r="O79" t="s">
         <v>247</v>
       </c>
+      <c r="P79" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="I80" t="s">
@@ -3976,6 +4096,9 @@
       <c r="O80" t="s">
         <v>254</v>
       </c>
+      <c r="P80" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="81" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I81" t="s">
@@ -3984,6 +4107,9 @@
       <c r="O81" t="s">
         <v>253</v>
       </c>
+      <c r="P81" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="82" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I82" t="s">
@@ -3992,6 +4118,9 @@
       <c r="O82" t="s">
         <v>251</v>
       </c>
+      <c r="P82" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="83" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I83" t="s">
@@ -4000,6 +4129,9 @@
       <c r="O83" t="s">
         <v>252</v>
       </c>
+      <c r="P83" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="84" spans="9:16" x14ac:dyDescent="0.35">
       <c r="I84" t="s">
@@ -4155,12 +4287,12 @@
       </c>
       <c r="P99" s="2">
         <f>SUM(P2:P98)</f>
-        <v>70</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M49:N55">
-    <sortCondition ref="M49:M55"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M50:N56">
+    <sortCondition ref="M50:M56"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="A53:C53"/>

</xml_diff>

<commit_message>
Rounded out forms support- still want to refactor a bit, but this gets some words down on the page.
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\coding\dotPDFium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFC3F9B-FCCA-4777-B3D3-A28415ECF6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F334D3-57E0-4D4D-8AD8-B843A5B7E894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39600" yWindow="620" windowWidth="36190" windowHeight="19510" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
+    <workbookView xWindow="40260" yWindow="790" windowWidth="36190" windowHeight="19510" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="446">
   <si>
     <t>Text_LoadPage</t>
   </si>
@@ -302,12 +302,6 @@
     <t>Dest_GetDestPageIndex</t>
   </si>
   <si>
-    <t>_GetMetaText</t>
-  </si>
-  <si>
-    <t>_GetPageLabel</t>
-  </si>
-  <si>
     <t>Link_GetLinkAtPoint</t>
   </si>
   <si>
@@ -401,15 +395,9 @@
     <t>FORM_DoDocumentOpenAction</t>
   </si>
   <si>
-    <t>_FFLDraw</t>
-  </si>
-  <si>
     <t>_GetFormType</t>
   </si>
   <si>
-    <t>_LoadXFA</t>
-  </si>
-  <si>
     <t>_ImportPagesByIndex</t>
   </si>
   <si>
@@ -1049,18 +1037,12 @@
     <t>FFLDraw</t>
   </si>
   <si>
-    <t>GetFormType</t>
-  </si>
-  <si>
     <t>LoadXFA</t>
   </si>
   <si>
     <t>FORM_OnFocus</t>
   </si>
   <si>
-    <t>FORM_OnButtonDown</t>
-  </si>
-  <si>
     <t>FORM_OnChar</t>
   </si>
   <si>
@@ -1233,6 +1215,165 @@
   </si>
   <si>
     <t>GetDocUserPermissions</t>
+  </si>
+  <si>
+    <t>Annot_IsObjectSupportedSubtype</t>
+  </si>
+  <si>
+    <t>Annot_UpdateObject</t>
+  </si>
+  <si>
+    <t>Annot_AddInkStroke</t>
+  </si>
+  <si>
+    <t>Annot_RemoveInkList</t>
+  </si>
+  <si>
+    <t>Annot_AppendObject</t>
+  </si>
+  <si>
+    <t>Annot_GetObjectCount</t>
+  </si>
+  <si>
+    <t>Annot_GetObject</t>
+  </si>
+  <si>
+    <t>Annot_RemoveObject</t>
+  </si>
+  <si>
+    <t>Annot_HasAttachmentPoints</t>
+  </si>
+  <si>
+    <t>Annot_SetAttachmentPoints</t>
+  </si>
+  <si>
+    <t>Annot_CountAttachmentPoints</t>
+  </si>
+  <si>
+    <t>Annot_GetAttachmentPoints</t>
+  </si>
+  <si>
+    <t>Annot_GetVertices</t>
+  </si>
+  <si>
+    <t>Annot_GetInkListCount</t>
+  </si>
+  <si>
+    <t>Annot_GetInkListPath</t>
+  </si>
+  <si>
+    <t>Annot_GetLine</t>
+  </si>
+  <si>
+    <t>Annot_SetBorder</t>
+  </si>
+  <si>
+    <t>Annot_GetBorder</t>
+  </si>
+  <si>
+    <t>Annot_HasKey</t>
+  </si>
+  <si>
+    <t>Annot_GetValueType</t>
+  </si>
+  <si>
+    <t>Annot_GetStringValue</t>
+  </si>
+  <si>
+    <t>Annot_GetNumberValue</t>
+  </si>
+  <si>
+    <t>Annot_SetAP</t>
+  </si>
+  <si>
+    <t>Annot_GetAP</t>
+  </si>
+  <si>
+    <t>Annot_GetLinkedAnnot</t>
+  </si>
+  <si>
+    <t>Annot_GetFlags</t>
+  </si>
+  <si>
+    <t>Annot_SetFlags</t>
+  </si>
+  <si>
+    <t>Annot_GetFileAttachment</t>
+  </si>
+  <si>
+    <t>Annot_AddFileAttachment</t>
+  </si>
+  <si>
+    <t>Annot_SetURI</t>
+  </si>
+  <si>
+    <t>Annot_GetFormFieldAtPoint</t>
+  </si>
+  <si>
+    <t>Annot_GetFormFieldName</t>
+  </si>
+  <si>
+    <t>Annot_GetFormFieldAlternateName</t>
+  </si>
+  <si>
+    <t>Annot_GetFormFieldType</t>
+  </si>
+  <si>
+    <t>Annot_GetFormFieldValue</t>
+  </si>
+  <si>
+    <t>Annot_GetFormFieldExportValue</t>
+  </si>
+  <si>
+    <t>Annot_GetFormFieldFlags</t>
+  </si>
+  <si>
+    <t>Annot_GetOptionCount</t>
+  </si>
+  <si>
+    <t>Annot_GetOptionLabel</t>
+  </si>
+  <si>
+    <t>Annot_IsOptionSelected</t>
+  </si>
+  <si>
+    <t>Annot_GetFontSize</t>
+  </si>
+  <si>
+    <t>Annot_GetFontColor</t>
+  </si>
+  <si>
+    <t>Annot_IsChecked</t>
+  </si>
+  <si>
+    <t>Annot_SetFocusableSubtypes</t>
+  </si>
+  <si>
+    <t>Annot_GetFocusableSubtypesCount</t>
+  </si>
+  <si>
+    <t>Annot_GetFocusableSubtypes</t>
+  </si>
+  <si>
+    <t>Annot_GetFormAdditionalActionJavaScript</t>
+  </si>
+  <si>
+    <t>Annot_GetFormControlCount</t>
+  </si>
+  <si>
+    <t>Annot_GetFormControlIndex</t>
+  </si>
+  <si>
+    <t>Annot_SetStringValue</t>
+  </si>
+  <si>
+    <t>FORM_OnLButtonDown</t>
+  </si>
+  <si>
+    <t>FORM_OnLButtonUp</t>
+  </si>
+  <si>
+    <t>FORM_SetFocusedAnnot</t>
   </si>
 </sst>
 </file>
@@ -1700,7 +1841,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93991F7-7A9D-4291-8EC0-AB472EBDEDBD}">
-  <dimension ref="A1:R99"/>
+  <dimension ref="A1:R103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1710,7 +1851,7 @@
     <col min="2" max="2" width="7.36328125" style="2" customWidth="1"/>
     <col min="3" max="3" width="36.08984375" customWidth="1"/>
     <col min="4" max="4" width="8.26953125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.90625" customWidth="1"/>
+    <col min="5" max="5" width="35.6328125" customWidth="1"/>
     <col min="6" max="6" width="3.81640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="37.1796875" customWidth="1"/>
     <col min="8" max="8" width="3.90625" style="2" customWidth="1"/>
@@ -1728,36 +1869,36 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="O1" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>316</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -1769,7 +1910,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>421</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
@@ -1787,16 +1928,19 @@
         <v>68</v>
       </c>
       <c r="M2" t="s">
-        <v>88</v>
+        <v>84</v>
+      </c>
+      <c r="N2" s="2">
+        <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="P2" s="2">
         <v>1</v>
       </c>
       <c r="Q2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="R2" s="2">
         <v>1</v>
@@ -1804,7 +1948,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -1816,13 +1960,13 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>395</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="H3" s="2">
         <v>1</v>
@@ -1834,16 +1978,19 @@
         <v>69</v>
       </c>
       <c r="M3" t="s">
-        <v>89</v>
+        <v>85</v>
+      </c>
+      <c r="N3" s="2">
+        <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
       </c>
       <c r="Q3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="R3" s="2">
         <v>1</v>
@@ -1851,7 +1998,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
@@ -1863,7 +2010,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>397</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
@@ -1885,19 +2032,19 @@
         <v>71</v>
       </c>
       <c r="M4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N4" s="2">
         <v>1</v>
       </c>
       <c r="O4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="P4" s="2">
         <v>1</v>
       </c>
       <c r="Q4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="R4" s="2">
         <v>1</v>
@@ -1905,7 +2052,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
@@ -1917,7 +2064,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>403</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
@@ -1932,19 +2079,19 @@
         <v>75</v>
       </c>
       <c r="M5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N5" s="2">
         <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="P5" s="2">
         <v>1</v>
       </c>
       <c r="Q5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="R5" s="2">
         <v>1</v>
@@ -1952,7 +2099,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
@@ -1964,7 +2111,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>416</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
@@ -1979,19 +2126,19 @@
         <v>70</v>
       </c>
       <c r="M6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N6" s="2">
         <v>1</v>
       </c>
       <c r="O6" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="P6" s="2">
         <v>1</v>
       </c>
       <c r="Q6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R6" s="2">
         <v>1</v>
@@ -1999,7 +2146,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
@@ -2011,7 +2158,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>404</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
@@ -2026,19 +2173,19 @@
         <v>73</v>
       </c>
       <c r="M7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="N7" s="2">
         <v>1</v>
       </c>
       <c r="O7" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="P7" s="2">
         <v>1</v>
       </c>
       <c r="Q7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="R7" s="2">
         <v>1</v>
@@ -2046,7 +2193,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
@@ -2058,7 +2205,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>410</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
@@ -2073,13 +2220,13 @@
         <v>74</v>
       </c>
       <c r="M8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N8" s="2">
         <v>1</v>
       </c>
       <c r="O8" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="P8" s="2">
         <v>1</v>
@@ -2106,7 +2253,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
@@ -2121,13 +2268,13 @@
         <v>72</v>
       </c>
       <c r="M9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N9" s="2">
         <v>1</v>
       </c>
       <c r="O9" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="P9" s="2">
         <v>1</v>
@@ -2147,7 +2294,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>420</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
@@ -2166,13 +2313,13 @@
         <v>0</v>
       </c>
       <c r="M10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="N10" s="2">
         <v>1</v>
       </c>
       <c r="O10" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="P10" s="2">
         <v>1</v>
@@ -2192,7 +2339,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>418</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
@@ -2204,13 +2351,13 @@
         <v>1</v>
       </c>
       <c r="M11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="N11" s="2">
         <v>1</v>
       </c>
       <c r="O11" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="P11" s="2">
         <v>1</v>
@@ -2230,7 +2377,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>438</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
@@ -2242,13 +2389,13 @@
         <v>1</v>
       </c>
       <c r="M12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="N12" s="2">
         <v>1</v>
       </c>
       <c r="O12" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="P12" s="2">
         <v>1</v>
@@ -2262,13 +2409,13 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>49</v>
+        <v>437</v>
       </c>
       <c r="F13" s="2">
         <v>1</v>
@@ -2280,13 +2427,13 @@
         <v>1</v>
       </c>
       <c r="M13" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="N13" s="2">
         <v>1</v>
       </c>
       <c r="O13" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="P13" s="2">
         <v>1</v>
@@ -2305,12 +2452,11 @@
       <c r="D14" s="2">
         <v>1</v>
       </c>
-      <c r="E14" s="4">
-        <v>12</v>
+      <c r="E14" t="s">
+        <v>434</v>
       </c>
       <c r="F14" s="2">
-        <f>SUM(F2:F13)</f>
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G14" s="4">
         <v>12</v>
@@ -2320,13 +2466,13 @@
         <v>12</v>
       </c>
       <c r="M14" t="s">
-        <v>78</v>
+        <v>324</v>
       </c>
       <c r="N14" s="2">
         <v>1</v>
       </c>
       <c r="O14" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="P14" s="2">
         <v>1</v>
@@ -2345,14 +2491,20 @@
       <c r="D15" s="2">
         <v>1</v>
       </c>
+      <c r="E15" t="s">
+        <v>433</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
       <c r="M15" t="s">
-        <v>87</v>
+        <v>391</v>
       </c>
       <c r="N15" s="2">
         <v>1</v>
       </c>
       <c r="O15" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="P15" s="2">
         <v>1</v>
@@ -2366,39 +2518,51 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>293</v>
+        <v>289</v>
+      </c>
+      <c r="E16" t="s">
+        <v>439</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
       </c>
       <c r="M16" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="N16" s="2">
         <v>1</v>
       </c>
       <c r="O16" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D17" s="2">
         <v>1</v>
       </c>
+      <c r="E17" t="s">
+        <v>440</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
       <c r="M17" t="s">
-        <v>397</v>
+        <v>326</v>
       </c>
       <c r="N17" s="2">
         <v>1</v>
       </c>
       <c r="O17" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
@@ -2409,9 +2573,15 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>441</v>
+      </c>
+      <c r="F18" s="2">
         <v>1</v>
       </c>
       <c r="M18" t="s">
@@ -2421,7 +2591,7 @@
         <v>1</v>
       </c>
       <c r="O18" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="P18" s="2">
         <v>1</v>
@@ -2435,16 +2605,25 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
       </c>
+      <c r="E19" t="s">
+        <v>425</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
       <c r="M19" t="s">
-        <v>330</v>
+        <v>325</v>
+      </c>
+      <c r="N19" s="2">
+        <v>1</v>
       </c>
       <c r="O19" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="P19" s="2">
         <v>1</v>
@@ -2463,11 +2642,20 @@
       <c r="D20" s="2">
         <v>1</v>
       </c>
+      <c r="E20" t="s">
+        <v>423</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
       <c r="M20" t="s">
-        <v>331</v>
+        <v>328</v>
+      </c>
+      <c r="N20" s="2">
+        <v>1</v>
       </c>
       <c r="O20" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="P20" s="2">
         <v>1</v>
@@ -2475,22 +2663,31 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B21" s="2">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
       </c>
+      <c r="E21" t="s">
+        <v>428</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
       <c r="M21" t="s">
-        <v>329</v>
+        <v>321</v>
+      </c>
+      <c r="N21" s="2">
+        <v>1</v>
       </c>
       <c r="O21" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="P21" s="2">
         <v>1</v>
@@ -2498,22 +2695,31 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B22" s="2">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D22" s="2">
         <v>1</v>
       </c>
+      <c r="E22" t="s">
+        <v>429</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1</v>
+      </c>
       <c r="M22" t="s">
-        <v>332</v>
+        <v>318</v>
+      </c>
+      <c r="N22" s="2">
+        <v>1</v>
       </c>
       <c r="O22" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="P22" s="2">
         <v>1</v>
@@ -2521,25 +2727,31 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B23" s="2">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D23" s="2">
         <v>1</v>
       </c>
+      <c r="E23" t="s">
+        <v>424</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
       <c r="M23" t="s">
-        <v>325</v>
+        <v>91</v>
       </c>
       <c r="N23" s="2">
         <v>1</v>
       </c>
       <c r="O23" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="P23" s="2">
         <v>1</v>
@@ -2547,7 +2759,7 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B24" s="2">
         <v>1</v>
@@ -2558,14 +2770,20 @@
       <c r="D24" s="2">
         <v>1</v>
       </c>
+      <c r="E24" t="s">
+        <v>426</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1</v>
+      </c>
       <c r="M24" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="N24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O24" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="P24" s="2">
         <v>1</v>
@@ -2573,7 +2791,7 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B25" s="2">
         <v>1</v>
@@ -2584,14 +2802,20 @@
       <c r="D25" s="2">
         <v>1</v>
       </c>
+      <c r="E25" t="s">
+        <v>427</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
       <c r="M25" t="s">
-        <v>93</v>
+        <v>320</v>
       </c>
       <c r="N25" s="2">
         <v>1</v>
       </c>
       <c r="O25" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="P25" s="2">
         <v>1</v>
@@ -2599,7 +2823,7 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
@@ -2610,14 +2834,20 @@
       <c r="D26" s="2">
         <v>1</v>
       </c>
+      <c r="E26" t="s">
+        <v>406</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1</v>
+      </c>
       <c r="M26" t="s">
-        <v>323</v>
+        <v>90</v>
       </c>
       <c r="N26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O26" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="P26" s="2">
         <v>1</v>
@@ -2625,25 +2855,31 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B27" s="2">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D27" s="2">
         <v>1</v>
       </c>
+      <c r="E27" t="s">
+        <v>407</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1</v>
+      </c>
       <c r="M27" t="s">
-        <v>324</v>
+        <v>88</v>
       </c>
       <c r="N27" s="2">
         <v>1</v>
       </c>
       <c r="O27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="P27" s="2">
         <v>1</v>
@@ -2657,19 +2893,25 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D28" s="2">
         <v>1</v>
       </c>
+      <c r="E28" t="s">
+        <v>408</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
       <c r="M28" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="N28" s="2">
         <v>1</v>
       </c>
       <c r="O28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="P28" s="2">
         <v>1</v>
@@ -2688,8 +2930,12 @@
       <c r="D29" s="2">
         <v>1</v>
       </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="3"/>
+      <c r="E29" t="s">
+        <v>417</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1</v>
+      </c>
       <c r="G29" s="1"/>
       <c r="H29" s="3"/>
       <c r="I29" s="1"/>
@@ -2697,13 +2943,13 @@
       <c r="K29" s="1"/>
       <c r="L29" s="3"/>
       <c r="M29" t="s">
-        <v>90</v>
+        <v>322</v>
       </c>
       <c r="N29" s="2">
         <v>1</v>
       </c>
       <c r="O29" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="P29" s="2">
         <v>1</v>
@@ -2711,9 +2957,9 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="3"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B30" s="2">
         <v>1</v>
@@ -2724,32 +2970,36 @@
       <c r="D30" s="2">
         <v>1</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>369</v>
+      <c r="E30" t="s">
+        <v>414</v>
+      </c>
+      <c r="F30" s="2">
+        <v>1</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>372</v>
-      </c>
-      <c r="M30" t="s">
-        <v>91</v>
-      </c>
-      <c r="N30" s="2">
-        <v>1</v>
+        <v>366</v>
+      </c>
+      <c r="M30" s="8">
+        <v>28</v>
+      </c>
+      <c r="N30" s="3">
+        <f>SUM(N2:N29)</f>
+        <v>27</v>
       </c>
       <c r="O30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="P30" s="2">
         <v>1</v>
       </c>
       <c r="Q30" s="6" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.35">
@@ -2760,85 +3010,84 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E31" t="s">
-        <v>128</v>
+        <v>399</v>
+      </c>
+      <c r="F31" s="2">
+        <v>1</v>
       </c>
       <c r="G31" t="s">
+        <v>130</v>
+      </c>
+      <c r="I31" t="s">
+        <v>131</v>
+      </c>
+      <c r="J31" s="2">
+        <v>1</v>
+      </c>
+      <c r="K31" t="s">
+        <v>133</v>
+      </c>
+      <c r="L31" s="2">
+        <v>1</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="O31" t="s">
+        <v>196</v>
+      </c>
+      <c r="P31" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="7" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>269</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>290</v>
+      </c>
+      <c r="E32" t="s">
+        <v>398</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
+      <c r="G32" t="s">
+        <v>129</v>
+      </c>
+      <c r="I32" t="s">
+        <v>132</v>
+      </c>
+      <c r="J32" s="2">
+        <v>1</v>
+      </c>
+      <c r="K32" t="s">
         <v>134</v>
       </c>
-      <c r="I31" t="s">
+      <c r="L32" s="2">
+        <v>1</v>
+      </c>
+      <c r="M32" t="s">
         <v>135</v>
       </c>
-      <c r="J31" s="2">
-        <v>1</v>
-      </c>
-      <c r="K31" t="s">
-        <v>137</v>
-      </c>
-      <c r="L31" s="2">
-        <v>1</v>
-      </c>
-      <c r="M31" t="s">
-        <v>326</v>
-      </c>
-      <c r="N31" s="2">
-        <v>1</v>
-      </c>
-      <c r="O31" t="s">
-        <v>200</v>
-      </c>
-      <c r="P31" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q31" s="7" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
-        <v>273</v>
-      </c>
-      <c r="B32" s="2">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>294</v>
-      </c>
-      <c r="E32" t="s">
-        <v>130</v>
-      </c>
-      <c r="G32" t="s">
-        <v>133</v>
-      </c>
-      <c r="I32" t="s">
-        <v>136</v>
-      </c>
-      <c r="J32" s="2">
-        <v>1</v>
-      </c>
-      <c r="K32" t="s">
-        <v>138</v>
-      </c>
-      <c r="L32" s="2">
-        <v>1</v>
-      </c>
-      <c r="M32" s="8">
-        <v>30</v>
-      </c>
-      <c r="N32" s="3">
-        <f>SUM(N2:N31)</f>
-        <v>23</v>
-      </c>
       <c r="O32" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="P32" s="2">
         <v>1</v>
       </c>
       <c r="Q32" s="7" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
@@ -2849,13 +3098,16 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E33" t="s">
-        <v>126</v>
+        <v>430</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I33" s="4">
         <v>2</v>
@@ -2871,60 +3123,66 @@
         <f>SUM(L31:L32)</f>
         <v>2</v>
       </c>
-      <c r="M33" s="6" t="s">
-        <v>373</v>
+      <c r="M33" t="s">
+        <v>136</v>
       </c>
       <c r="O33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="P33" s="2">
         <v>1</v>
       </c>
       <c r="Q33" s="7" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B34" s="2">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E34" t="s">
-        <v>125</v>
+        <v>431</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="M34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="O34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="P34" s="2">
         <v>1</v>
       </c>
       <c r="Q34" s="7" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B35" s="2">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E35" t="s">
-        <v>124</v>
+        <v>54</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1</v>
       </c>
       <c r="G35" s="4">
         <v>4</v>
@@ -2934,21 +3192,21 @@
         <v>0</v>
       </c>
       <c r="M35" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="O35" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="P35" s="2">
         <v>1</v>
       </c>
       <c r="Q35" s="7" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B36" s="2">
         <v>1</v>
@@ -2960,19 +3218,22 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>129</v>
+        <v>413</v>
+      </c>
+      <c r="F36" s="2">
+        <v>1</v>
       </c>
       <c r="M36" t="s">
         <v>142</v>
       </c>
       <c r="O36" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="P36" s="2">
         <v>1</v>
       </c>
       <c r="Q36" s="7" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
@@ -2983,25 +3244,28 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D37" s="2">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>127</v>
+        <v>50</v>
+      </c>
+      <c r="F37" s="2">
+        <v>1</v>
       </c>
       <c r="M37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O37" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="P37" s="2">
         <v>1</v>
       </c>
       <c r="Q37" s="7" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.35">
@@ -3018,24 +3282,23 @@
       <c r="D38" s="2">
         <v>1</v>
       </c>
-      <c r="E38" s="4">
-        <v>7</v>
+      <c r="E38" t="s">
+        <v>412</v>
       </c>
       <c r="F38" s="2">
-        <f>SUM(F31:F37)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M38" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="O38" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="P38" s="2">
         <v>1</v>
       </c>
       <c r="Q38" s="7" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
@@ -3045,17 +3308,23 @@
       <c r="D39" s="2">
         <v>1</v>
       </c>
+      <c r="E39" t="s">
+        <v>405</v>
+      </c>
+      <c r="F39" s="2">
+        <v>1</v>
+      </c>
       <c r="M39" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="O39" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="P39" s="2">
         <v>1</v>
       </c>
       <c r="Q39" s="7" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
@@ -3065,17 +3334,27 @@
       <c r="D40" s="2">
         <v>1</v>
       </c>
-      <c r="M40" t="s">
-        <v>143</v>
+      <c r="E40" t="s">
+        <v>401</v>
+      </c>
+      <c r="F40" s="2">
+        <v>1</v>
+      </c>
+      <c r="M40" s="4">
+        <v>8</v>
+      </c>
+      <c r="N40" s="2">
+        <f>SUM(N32:N39)</f>
+        <v>0</v>
       </c>
       <c r="O40" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="P40" s="2">
         <v>1</v>
       </c>
       <c r="Q40" s="7" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
@@ -3085,17 +3364,20 @@
       <c r="D41" s="2">
         <v>1</v>
       </c>
-      <c r="M41" t="s">
-        <v>145</v>
+      <c r="E41" t="s">
+        <v>411</v>
+      </c>
+      <c r="F41" s="2">
+        <v>1</v>
       </c>
       <c r="O41" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="P41" s="2">
         <v>1</v>
       </c>
       <c r="Q41" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.35">
@@ -3105,21 +3387,20 @@
       <c r="D42" s="2">
         <v>1</v>
       </c>
-      <c r="M42" s="4">
-        <v>8</v>
-      </c>
-      <c r="N42" s="2">
-        <f>SUM(N34:N41)</f>
-        <v>0</v>
+      <c r="E42" t="s">
+        <v>435</v>
+      </c>
+      <c r="F42" s="2">
+        <v>1</v>
       </c>
       <c r="O42" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="P42" s="2">
         <v>1</v>
       </c>
       <c r="Q42" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.35">
@@ -3129,14 +3410,20 @@
       <c r="D43" s="2">
         <v>1</v>
       </c>
+      <c r="E43" t="s">
+        <v>393</v>
+      </c>
+      <c r="F43" s="2">
+        <v>1</v>
+      </c>
       <c r="O43" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="P43" s="2">
         <v>1</v>
       </c>
       <c r="Q43" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
@@ -3146,142 +3433,185 @@
       <c r="D44" s="2">
         <v>1</v>
       </c>
+      <c r="E44" t="s">
+        <v>432</v>
+      </c>
+      <c r="F44" s="2">
+        <v>1</v>
+      </c>
       <c r="O44" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="P44" s="2">
         <v>1</v>
       </c>
       <c r="Q44" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C45" t="s">
-        <v>305</v>
+        <v>301</v>
+      </c>
+      <c r="E45" t="s">
+        <v>43</v>
+      </c>
+      <c r="F45" s="2">
+        <v>1</v>
       </c>
       <c r="O45" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="Q45" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C46" t="s">
-        <v>306</v>
-      </c>
+        <v>302</v>
+      </c>
+      <c r="E46" t="s">
+        <v>396</v>
+      </c>
+      <c r="F46" s="2">
+        <v>1</v>
+      </c>
+      <c r="M46" s="1"/>
       <c r="O46" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="Q46" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="1"/>
       <c r="B47" s="3"/>
       <c r="C47" t="s">
-        <v>301</v>
-      </c>
-      <c r="E47" s="1"/>
-      <c r="F47" s="3"/>
+        <v>297</v>
+      </c>
+      <c r="E47" t="s">
+        <v>400</v>
+      </c>
+      <c r="F47" s="2">
+        <v>1</v>
+      </c>
       <c r="G47" s="1"/>
       <c r="H47" s="3"/>
       <c r="I47" s="1"/>
       <c r="J47" s="3"/>
       <c r="K47" s="1"/>
       <c r="L47" s="3"/>
+      <c r="M47" s="5" t="s">
+        <v>384</v>
+      </c>
       <c r="O47" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="Q47" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C48" t="s">
-        <v>302</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>393</v>
+        <v>298</v>
+      </c>
+      <c r="E48" t="s">
+        <v>415</v>
+      </c>
+      <c r="F48" s="2">
+        <v>1</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="M48" s="1"/>
+        <v>317</v>
+      </c>
+      <c r="M48" t="s">
+        <v>161</v>
+      </c>
+      <c r="N48" s="2">
+        <v>1</v>
+      </c>
       <c r="O48" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="P48" s="2">
         <v>1</v>
       </c>
       <c r="Q48" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C49" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E49" t="s">
-        <v>187</v>
+        <v>402</v>
       </c>
       <c r="F49" s="2">
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="H49" s="2">
         <v>1</v>
       </c>
       <c r="I49" t="s">
-        <v>121</v>
+        <v>119</v>
+      </c>
+      <c r="J49" s="2">
+        <v>1</v>
       </c>
       <c r="K49" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L49" s="2">
         <v>1</v>
       </c>
-      <c r="M49" s="5" t="s">
-        <v>390</v>
+      <c r="M49" t="s">
+        <v>160</v>
+      </c>
+      <c r="N49" s="2">
+        <v>1</v>
       </c>
       <c r="O49" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="P49" s="2">
         <v>1</v>
       </c>
       <c r="Q49" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C50" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E50" t="s">
-        <v>188</v>
+        <v>409</v>
       </c>
       <c r="F50" s="2">
         <v>1</v>
       </c>
       <c r="G50" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H50" s="2">
         <v>1</v>
       </c>
       <c r="I50" t="s">
-        <v>122</v>
+        <v>115</v>
+      </c>
+      <c r="J50" s="2">
+        <v>1</v>
       </c>
       <c r="K50" s="4">
         <v>1</v>
@@ -3291,48 +3621,51 @@
         <v>1</v>
       </c>
       <c r="M50" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="N50" s="2">
         <v>1</v>
       </c>
       <c r="O50" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="Q50" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C51" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E51" t="s">
-        <v>184</v>
+        <v>51</v>
       </c>
       <c r="F51" s="2">
         <v>1</v>
       </c>
       <c r="G51" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H51" s="2">
         <v>1</v>
       </c>
       <c r="I51" t="s">
-        <v>123</v>
+        <v>114</v>
+      </c>
+      <c r="J51" s="2">
+        <v>1</v>
       </c>
       <c r="M51" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="N51" s="2">
         <v>1</v>
       </c>
       <c r="O51" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="Q51" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.35">
@@ -3344,7 +3677,7 @@
         <v>37</v>
       </c>
       <c r="E52" t="s">
-        <v>185</v>
+        <v>419</v>
       </c>
       <c r="F52" s="2">
         <v>1</v>
@@ -3357,7 +3690,10 @@
         <v>3</v>
       </c>
       <c r="I52" t="s">
-        <v>117</v>
+        <v>332</v>
+      </c>
+      <c r="J52" s="2">
+        <v>1</v>
       </c>
       <c r="M52" t="s">
         <v>163</v>
@@ -3366,102 +3702,112 @@
         <v>1</v>
       </c>
       <c r="O52" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="P52" s="2">
         <v>1</v>
       </c>
       <c r="Q52" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E53" t="s">
-        <v>186</v>
+        <v>436</v>
       </c>
       <c r="F53" s="2">
         <v>1</v>
       </c>
       <c r="I53" t="s">
-        <v>116</v>
+        <v>351</v>
+      </c>
+      <c r="J53" s="2">
+        <v>1</v>
       </c>
       <c r="M53" t="s">
-        <v>166</v>
+        <v>385</v>
       </c>
       <c r="N53" s="2">
         <v>1</v>
       </c>
       <c r="O53" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="P53" s="2">
         <v>1</v>
       </c>
       <c r="Q53" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.35">
       <c r="E54" t="s">
-        <v>180</v>
+        <v>53</v>
       </c>
       <c r="F54" s="2">
         <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>336</v>
+        <v>350</v>
+      </c>
+      <c r="J54" s="2">
+        <v>1</v>
       </c>
       <c r="M54" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="N54" s="2">
         <v>1</v>
       </c>
       <c r="O54" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="P54" s="2">
         <v>1</v>
       </c>
       <c r="Q54" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A55" s="15" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="B55" s="15"/>
       <c r="C55" s="15"/>
       <c r="D55" s="11"/>
       <c r="E55" t="s">
-        <v>178</v>
+        <v>442</v>
       </c>
       <c r="F55" s="2">
         <v>1</v>
       </c>
       <c r="I55" t="s">
-        <v>357</v>
-      </c>
-      <c r="M55" t="s">
-        <v>391</v>
+        <v>338</v>
+      </c>
+      <c r="J55" s="2">
+        <v>1</v>
+      </c>
+      <c r="M55" s="4">
+        <v>7</v>
       </c>
       <c r="N55" s="2">
-        <v>1</v>
+        <f>SUM(N48:N54)</f>
+        <v>7</v>
       </c>
       <c r="O55" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="P55" s="2">
         <v>1</v>
       </c>
       <c r="Q55" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A56" s="10" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B56" s="9">
         <f>A38</f>
@@ -3476,33 +3822,30 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>177</v>
+        <v>422</v>
       </c>
       <c r="F56" s="2">
         <v>1</v>
       </c>
       <c r="I56" t="s">
-        <v>356</v>
-      </c>
-      <c r="M56" t="s">
-        <v>162</v>
-      </c>
-      <c r="N56" s="2">
+        <v>117</v>
+      </c>
+      <c r="J56" s="2">
         <v>1</v>
       </c>
       <c r="O56" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="P56" s="2">
         <v>1</v>
       </c>
       <c r="Q56" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A57" s="10" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B57" s="9">
         <f>C52</f>
@@ -3517,69 +3860,68 @@
         <v>0.74</v>
       </c>
       <c r="E57" t="s">
-        <v>176</v>
+        <v>394</v>
       </c>
       <c r="F57" s="2">
         <v>1</v>
       </c>
       <c r="I57" t="s">
-        <v>344</v>
-      </c>
-      <c r="M57" s="4">
-        <v>7</v>
-      </c>
-      <c r="N57" s="2">
-        <f>SUM(N50:N56)</f>
-        <v>7</v>
+        <v>118</v>
+      </c>
+      <c r="J57" s="2">
+        <v>1</v>
       </c>
       <c r="O57" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="P57" s="2">
         <v>1</v>
       </c>
       <c r="Q57" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A58" s="10" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B58" s="9">
-        <f>E14</f>
-        <v>12</v>
+        <f>E64</f>
+        <v>62</v>
       </c>
       <c r="C58" s="12">
-        <f>F14</f>
-        <v>12</v>
+        <f>F64</f>
+        <v>61</v>
       </c>
       <c r="D58" s="16">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.9838709677419355</v>
       </c>
       <c r="E58" t="s">
-        <v>179</v>
+        <v>48</v>
       </c>
       <c r="F58" s="2">
         <v>1</v>
       </c>
       <c r="I58" t="s">
-        <v>119</v>
+        <v>339</v>
+      </c>
+      <c r="J58" s="2">
+        <v>1</v>
       </c>
       <c r="O58" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="P58" s="2">
         <v>1</v>
       </c>
       <c r="Q58" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A59" s="10" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B59" s="9">
         <f>G14</f>
@@ -3594,27 +3936,30 @@
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>189</v>
+        <v>44</v>
       </c>
       <c r="F59" s="2">
         <v>1</v>
       </c>
       <c r="I59" t="s">
-        <v>120</v>
+        <v>354</v>
+      </c>
+      <c r="J59" s="2">
+        <v>1</v>
       </c>
       <c r="O59" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="P59" s="2">
         <v>1</v>
       </c>
       <c r="Q59" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A60" s="10" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B60" s="9">
         <f>I4</f>
@@ -3629,27 +3974,30 @@
         <v>0</v>
       </c>
       <c r="E60" t="s">
-        <v>175</v>
+        <v>46</v>
       </c>
       <c r="F60" s="2">
         <v>1</v>
       </c>
       <c r="I60" t="s">
-        <v>345</v>
+        <v>355</v>
+      </c>
+      <c r="J60" s="2">
+        <v>1</v>
       </c>
       <c r="O60" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="P60" s="2">
         <v>1</v>
       </c>
       <c r="Q60" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="10" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B61" s="9">
         <f>K10</f>
@@ -3664,16 +4012,19 @@
         <v>0</v>
       </c>
       <c r="E61" t="s">
-        <v>173</v>
+        <v>45</v>
       </c>
       <c r="F61" s="2">
         <v>1</v>
       </c>
       <c r="I61" t="s">
-        <v>360</v>
+        <v>345</v>
+      </c>
+      <c r="J61" s="2">
+        <v>1</v>
       </c>
       <c r="O61" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="P61" s="2">
         <v>1</v>
@@ -3688,36 +4039,39 @@
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A62" s="10" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B62" s="9">
-        <f>M32</f>
-        <v>30</v>
+        <f>M30</f>
+        <v>28</v>
       </c>
       <c r="C62" s="12">
-        <f>N32</f>
-        <v>23</v>
+        <f>N30</f>
+        <v>27</v>
       </c>
       <c r="D62" s="16">
         <f t="shared" si="0"/>
-        <v>0.76666666666666672</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="E62" t="s">
-        <v>172</v>
+        <v>47</v>
       </c>
       <c r="F62" s="2">
         <v>1</v>
       </c>
       <c r="I62" t="s">
-        <v>361</v>
+        <v>346</v>
+      </c>
+      <c r="J62" s="2">
+        <v>1</v>
       </c>
       <c r="O62" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A63" s="10" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="B63" s="9">
         <f>O99</f>
@@ -3732,21 +4086,24 @@
         <v>0.88659793814432986</v>
       </c>
       <c r="E63" t="s">
-        <v>171</v>
+        <v>49</v>
       </c>
       <c r="F63" s="2">
         <v>1</v>
       </c>
       <c r="I63" t="s">
-        <v>351</v>
+        <v>362</v>
+      </c>
+      <c r="J63" s="2">
+        <v>1</v>
       </c>
       <c r="O63" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="10" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B64" s="9">
         <f>Q8</f>
@@ -3760,17 +4117,21 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E64" t="s">
-        <v>174</v>
+      <c r="E64" s="4">
+        <v>62</v>
       </c>
       <c r="F64" s="2">
-        <v>1</v>
+        <f>SUM(F2:F63)</f>
+        <v>61</v>
       </c>
       <c r="I64" t="s">
-        <v>352</v>
+        <v>331</v>
+      </c>
+      <c r="J64" s="2">
+        <v>1</v>
       </c>
       <c r="O64" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="P64" s="2">
         <v>1</v>
@@ -3778,31 +4139,31 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="10" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="B65" s="9">
-        <f>E38</f>
+        <f>E73</f>
         <v>7</v>
       </c>
       <c r="C65" s="12">
-        <f>F38</f>
+        <f>F73</f>
         <v>0</v>
       </c>
       <c r="D65" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E65" t="s">
-        <v>181</v>
-      </c>
-      <c r="F65" s="2">
-        <v>1</v>
+      <c r="E65" s="6" t="s">
+        <v>363</v>
       </c>
       <c r="I65" t="s">
-        <v>368</v>
+        <v>116</v>
+      </c>
+      <c r="J65" s="2">
+        <v>1</v>
       </c>
       <c r="O65" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="P65" s="2">
         <v>1</v>
@@ -3810,7 +4171,7 @@
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="10" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="B66" s="9">
         <f>G35</f>
@@ -3825,21 +4186,21 @@
         <v>0</v>
       </c>
       <c r="E66" t="s">
-        <v>183</v>
-      </c>
-      <c r="F66" s="2">
-        <v>1</v>
+        <v>124</v>
       </c>
       <c r="I66" t="s">
         <v>335</v>
       </c>
+      <c r="J66" s="2">
+        <v>1</v>
+      </c>
       <c r="O66" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="10" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="B67" s="9">
         <f>I33</f>
@@ -3854,21 +4215,21 @@
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>182</v>
-      </c>
-      <c r="F67" s="2">
-        <v>1</v>
+        <v>126</v>
       </c>
       <c r="I67" t="s">
-        <v>118</v>
+        <v>334</v>
+      </c>
+      <c r="J67" s="2">
+        <v>1</v>
       </c>
       <c r="O67" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="10" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="B68" s="9">
         <f>K33</f>
@@ -3882,18 +4243,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E68" s="4">
-        <v>19</v>
-      </c>
-      <c r="F68" s="2">
-        <f>SUM(F49:F67)</f>
-        <v>19</v>
+      <c r="E68" t="s">
+        <v>122</v>
       </c>
       <c r="I68" t="s">
-        <v>340</v>
+        <v>336</v>
+      </c>
+      <c r="J68" s="2">
+        <v>1</v>
       </c>
       <c r="O68" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="P68" s="2">
         <v>1</v>
@@ -3901,25 +4261,31 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="10" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="B69" s="9">
-        <f>M42</f>
+        <f>M40</f>
         <v>8</v>
       </c>
       <c r="C69" s="12">
-        <f>N42</f>
+        <f>N40</f>
         <v>0</v>
       </c>
       <c r="D69" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="E69" t="s">
+        <v>121</v>
+      </c>
       <c r="I69" t="s">
-        <v>341</v>
+        <v>337</v>
+      </c>
+      <c r="J69" s="2">
+        <v>1</v>
       </c>
       <c r="O69" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="P69" s="2">
         <v>1</v>
@@ -3927,7 +4293,7 @@
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="10" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="B70" s="9">
         <f>Q61</f>
@@ -3941,11 +4307,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="E70" t="s">
+        <v>120</v>
+      </c>
       <c r="I70" t="s">
-        <v>339</v>
+        <v>344</v>
+      </c>
+      <c r="J70" s="2">
+        <v>1</v>
       </c>
       <c r="O70" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="P70" s="2">
         <v>1</v>
@@ -3953,25 +4325,31 @@
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="10" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="B71" s="9">
-        <f>E68</f>
+        <f>E103</f>
         <v>19</v>
       </c>
       <c r="C71" s="12">
-        <f>F68</f>
+        <f>F103</f>
         <v>19</v>
       </c>
       <c r="D71" s="16">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="E71" t="s">
+        <v>125</v>
+      </c>
       <c r="I71" t="s">
-        <v>342</v>
+        <v>443</v>
+      </c>
+      <c r="J71" s="2">
+        <v>1</v>
       </c>
       <c r="O71" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="P71" s="2">
         <v>1</v>
@@ -3979,7 +4357,7 @@
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" s="10" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="B72" s="9">
         <f>G52</f>
@@ -3993,11 +4371,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="E72" t="s">
+        <v>123</v>
+      </c>
       <c r="I72" t="s">
-        <v>343</v>
+        <v>444</v>
+      </c>
+      <c r="J72" s="2">
+        <v>1</v>
       </c>
       <c r="O72" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="P72" s="2">
         <v>1</v>
@@ -4005,25 +4389,35 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="10" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B73" s="9">
-        <f>I91</f>
-        <v>42</v>
+        <f>I90</f>
+        <v>41</v>
       </c>
       <c r="C73" s="12">
-        <f>J91</f>
-        <v>0</v>
+        <f>J90</f>
+        <v>40</v>
       </c>
       <c r="D73" s="16">
         <f t="shared" si="0"/>
+        <v>0.97560975609756095</v>
+      </c>
+      <c r="E73" s="4">
+        <v>7</v>
+      </c>
+      <c r="F73" s="2">
+        <f>SUM(F66:F72)</f>
         <v>0</v>
       </c>
       <c r="I73" t="s">
-        <v>350</v>
+        <v>340</v>
+      </c>
+      <c r="J73" s="2">
+        <v>1</v>
       </c>
       <c r="O73" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="P73" s="2">
         <v>1</v>
@@ -4031,7 +4425,7 @@
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" s="10" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B74" s="9">
         <f>K50</f>
@@ -4046,10 +4440,13 @@
         <v>1</v>
       </c>
       <c r="I74" t="s">
-        <v>346</v>
+        <v>341</v>
+      </c>
+      <c r="J74" s="2">
+        <v>1</v>
       </c>
       <c r="O74" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="P74" s="2">
         <v>1</v>
@@ -4057,14 +4454,14 @@
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" s="10" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="B75" s="9">
-        <f>M57</f>
+        <f>M55</f>
         <v>7</v>
       </c>
       <c r="C75" s="12">
-        <f>N57</f>
+        <f>N55</f>
         <v>7</v>
       </c>
       <c r="D75" s="16">
@@ -4072,10 +4469,13 @@
         <v>1</v>
       </c>
       <c r="I75" t="s">
-        <v>347</v>
+        <v>342</v>
+      </c>
+      <c r="J75" s="2">
+        <v>1</v>
       </c>
       <c r="O75" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="P75" s="2">
         <v>1</v>
@@ -4087,10 +4487,13 @@
       <c r="C76" s="12"/>
       <c r="D76" s="9"/>
       <c r="I76" t="s">
-        <v>348</v>
+        <v>343</v>
+      </c>
+      <c r="J76" s="2">
+        <v>1</v>
       </c>
       <c r="O76" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="P76" s="2">
         <v>1</v>
@@ -4100,18 +4503,21 @@
       <c r="A77" s="10"/>
       <c r="B77" s="9">
         <f>SUM(B56:B76)</f>
-        <v>377</v>
+        <v>424</v>
       </c>
       <c r="C77" s="12">
         <f>SUM(C56:C76)</f>
-        <v>246</v>
+        <v>339</v>
       </c>
       <c r="D77" s="9"/>
       <c r="I77" t="s">
-        <v>349</v>
+        <v>353</v>
+      </c>
+      <c r="J77" s="2">
+        <v>1</v>
       </c>
       <c r="O77" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="P77" s="2">
         <v>1</v>
@@ -4121,15 +4527,18 @@
       <c r="A78" s="13"/>
       <c r="B78" s="14">
         <f>C77/B77</f>
-        <v>0.65251989389920428</v>
+        <v>0.79952830188679247</v>
       </c>
       <c r="C78" s="13"/>
       <c r="D78" s="9"/>
       <c r="I78" t="s">
-        <v>359</v>
+        <v>347</v>
+      </c>
+      <c r="J78" s="2">
+        <v>1</v>
       </c>
       <c r="O78" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="P78" s="2">
         <v>1</v>
@@ -4137,10 +4546,13 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="I79" t="s">
-        <v>353</v>
+        <v>348</v>
+      </c>
+      <c r="J79" s="2">
+        <v>1</v>
       </c>
       <c r="O79" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="P79" s="2">
         <v>1</v>
@@ -4148,197 +4560,325 @@
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="I80" t="s">
-        <v>354</v>
+        <v>349</v>
+      </c>
+      <c r="J80" s="2">
+        <v>1</v>
       </c>
       <c r="O80" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="P80" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="9:16" x14ac:dyDescent="0.35">
+    <row r="81" spans="5:16" x14ac:dyDescent="0.35">
       <c r="I81" t="s">
-        <v>355</v>
+        <v>445</v>
+      </c>
+      <c r="J81" s="2">
+        <v>1</v>
       </c>
       <c r="O81" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="P81" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="9:16" x14ac:dyDescent="0.35">
+    <row r="82" spans="5:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E82" s="1"/>
+      <c r="F82" s="3"/>
       <c r="I82" t="s">
-        <v>367</v>
+        <v>361</v>
+      </c>
+      <c r="J82" s="2">
+        <v>1</v>
       </c>
       <c r="O82" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="P82" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="9:16" x14ac:dyDescent="0.35">
+    <row r="83" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E83" s="6" t="s">
+        <v>387</v>
+      </c>
       <c r="I83" t="s">
+        <v>352</v>
+      </c>
+      <c r="J83" s="2">
+        <v>1</v>
+      </c>
+      <c r="O83" t="s">
+        <v>248</v>
+      </c>
+      <c r="P83" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E84" t="s">
+        <v>183</v>
+      </c>
+      <c r="F84" s="2">
+        <v>1</v>
+      </c>
+      <c r="I84" t="s">
+        <v>333</v>
+      </c>
+      <c r="J84" s="2">
+        <v>0</v>
+      </c>
+      <c r="O84" t="s">
+        <v>211</v>
+      </c>
+      <c r="P84" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E85" t="s">
+        <v>184</v>
+      </c>
+      <c r="F85" s="2">
+        <v>1</v>
+      </c>
+      <c r="I85" t="s">
+        <v>357</v>
+      </c>
+      <c r="J85" s="2">
+        <v>1</v>
+      </c>
+      <c r="O85" t="s">
+        <v>213</v>
+      </c>
+      <c r="P85" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E86" t="s">
+        <v>180</v>
+      </c>
+      <c r="F86" s="2">
+        <v>1</v>
+      </c>
+      <c r="I86" t="s">
+        <v>356</v>
+      </c>
+      <c r="J86" s="2">
+        <v>1</v>
+      </c>
+      <c r="O86" t="s">
+        <v>210</v>
+      </c>
+      <c r="P86" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E87" t="s">
+        <v>181</v>
+      </c>
+      <c r="F87" s="2">
+        <v>1</v>
+      </c>
+      <c r="I87" t="s">
+        <v>360</v>
+      </c>
+      <c r="J87" s="2">
+        <v>1</v>
+      </c>
+      <c r="O87" t="s">
+        <v>209</v>
+      </c>
+      <c r="P87" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E88" t="s">
+        <v>182</v>
+      </c>
+      <c r="F88" s="2">
+        <v>1</v>
+      </c>
+      <c r="I88" t="s">
+        <v>359</v>
+      </c>
+      <c r="J88" s="2">
+        <v>1</v>
+      </c>
+      <c r="O88" t="s">
+        <v>212</v>
+      </c>
+      <c r="P88" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E89" t="s">
+        <v>176</v>
+      </c>
+      <c r="F89" s="2">
+        <v>1</v>
+      </c>
+      <c r="I89" t="s">
         <v>358</v>
       </c>
-      <c r="O83" t="s">
-        <v>252</v>
-      </c>
-      <c r="P83" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="9:16" x14ac:dyDescent="0.35">
-      <c r="I84" t="s">
-        <v>337</v>
-      </c>
-      <c r="O84" t="s">
+      <c r="J89" s="2">
+        <v>1</v>
+      </c>
+      <c r="O89" t="s">
+        <v>214</v>
+      </c>
+      <c r="P89" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E90" t="s">
+        <v>174</v>
+      </c>
+      <c r="F90" s="2">
+        <v>1</v>
+      </c>
+      <c r="I90" s="4">
+        <v>41</v>
+      </c>
+      <c r="J90" s="2">
+        <f>SUM(J49:J89)</f>
+        <v>40</v>
+      </c>
+      <c r="O90" t="s">
+        <v>188</v>
+      </c>
+      <c r="P90" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E91" t="s">
+        <v>173</v>
+      </c>
+      <c r="F91" s="2">
+        <v>1</v>
+      </c>
+      <c r="O91" t="s">
+        <v>104</v>
+      </c>
+      <c r="P91" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E92" t="s">
+        <v>172</v>
+      </c>
+      <c r="F92" s="2">
+        <v>1</v>
+      </c>
+      <c r="O92" t="s">
+        <v>103</v>
+      </c>
+      <c r="P92" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E93" t="s">
+        <v>175</v>
+      </c>
+      <c r="F93" s="2">
+        <v>1</v>
+      </c>
+      <c r="O93" t="s">
+        <v>220</v>
+      </c>
+      <c r="P93" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E94" t="s">
+        <v>185</v>
+      </c>
+      <c r="F94" s="2">
+        <v>1</v>
+      </c>
+      <c r="O94" t="s">
         <v>215</v>
       </c>
-      <c r="P84" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="9:16" x14ac:dyDescent="0.35">
-      <c r="I85" t="s">
-        <v>338</v>
-      </c>
-      <c r="O85" t="s">
+      <c r="P94" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E95" t="s">
+        <v>171</v>
+      </c>
+      <c r="F95" s="2">
+        <v>1</v>
+      </c>
+      <c r="O95" t="s">
+        <v>219</v>
+      </c>
+      <c r="P95" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E96" t="s">
+        <v>169</v>
+      </c>
+      <c r="F96" s="2">
+        <v>1</v>
+      </c>
+      <c r="O96" t="s">
+        <v>218</v>
+      </c>
+      <c r="P96" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E97" t="s">
+        <v>168</v>
+      </c>
+      <c r="F97" s="2">
+        <v>1</v>
+      </c>
+      <c r="O97" t="s">
         <v>217</v>
       </c>
-      <c r="P85" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="9:16" x14ac:dyDescent="0.35">
-      <c r="I86" t="s">
-        <v>363</v>
-      </c>
-      <c r="O86" t="s">
-        <v>214</v>
-      </c>
-      <c r="P86" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="9:16" x14ac:dyDescent="0.35">
-      <c r="I87" t="s">
-        <v>362</v>
-      </c>
-      <c r="O87" t="s">
-        <v>213</v>
-      </c>
-      <c r="P87" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="9:16" x14ac:dyDescent="0.35">
-      <c r="I88" t="s">
-        <v>366</v>
-      </c>
-      <c r="O88" t="s">
+      <c r="P97" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E98" t="s">
+        <v>167</v>
+      </c>
+      <c r="F98" s="2">
+        <v>1</v>
+      </c>
+      <c r="O98" t="s">
         <v>216</v>
       </c>
-      <c r="P88" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="9:16" x14ac:dyDescent="0.35">
-      <c r="I89" t="s">
-        <v>365</v>
-      </c>
-      <c r="O89" t="s">
-        <v>218</v>
-      </c>
-      <c r="P89" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="9:16" x14ac:dyDescent="0.35">
-      <c r="I90" t="s">
-        <v>364</v>
-      </c>
-      <c r="O90" t="s">
-        <v>192</v>
-      </c>
-      <c r="P90" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="9:16" x14ac:dyDescent="0.35">
-      <c r="I91" s="4">
-        <v>42</v>
-      </c>
-      <c r="J91" s="2">
-        <f>SUM(J49:J90)</f>
-        <v>0</v>
-      </c>
-      <c r="O91" t="s">
-        <v>106</v>
-      </c>
-      <c r="P91" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="9:16" x14ac:dyDescent="0.35">
-      <c r="O92" t="s">
-        <v>105</v>
-      </c>
-      <c r="P92" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="9:16" x14ac:dyDescent="0.35">
-      <c r="O93" t="s">
-        <v>224</v>
-      </c>
-      <c r="P93" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="9:16" x14ac:dyDescent="0.35">
-      <c r="O94" t="s">
-        <v>219</v>
-      </c>
-      <c r="P94" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="9:16" x14ac:dyDescent="0.35">
-      <c r="O95" t="s">
-        <v>223</v>
-      </c>
-      <c r="P95" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="9:16" x14ac:dyDescent="0.35">
-      <c r="O96" t="s">
-        <v>222</v>
-      </c>
-      <c r="P96" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="15:16" x14ac:dyDescent="0.35">
-      <c r="O97" t="s">
-        <v>221</v>
-      </c>
-      <c r="P97" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="15:16" x14ac:dyDescent="0.35">
-      <c r="O98" t="s">
-        <v>220</v>
-      </c>
       <c r="P98" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="15:16" x14ac:dyDescent="0.35">
+    <row r="99" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E99" t="s">
+        <v>170</v>
+      </c>
+      <c r="F99" s="2">
+        <v>1</v>
+      </c>
       <c r="O99" s="4">
         <v>97</v>
       </c>
@@ -4347,9 +4887,42 @@
         <v>86</v>
       </c>
     </row>
+    <row r="100" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E100" t="s">
+        <v>177</v>
+      </c>
+      <c r="F100" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E101" t="s">
+        <v>179</v>
+      </c>
+      <c r="F101" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E102" t="s">
+        <v>178</v>
+      </c>
+      <c r="F102" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E103" s="4">
+        <v>19</v>
+      </c>
+      <c r="F103" s="2">
+        <f>SUM(F84:F102)</f>
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M50:N56">
-    <sortCondition ref="M50:M56"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E2:F63">
+    <sortCondition ref="E2:E63"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="A55:C55"/>

</xml_diff>

<commit_message>
Added security and VIEWERREF_* functions.
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\coding\dotPDFium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F334D3-57E0-4D4D-8AD8-B843A5B7E894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D116886E-1BC5-4EBD-A323-BC81B1B4C344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40260" yWindow="790" windowWidth="36190" windowHeight="19510" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
   </bookViews>
@@ -1841,7 +1841,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93991F7-7A9D-4291-8EC0-AB472EBDEDBD}">
-  <dimension ref="A1:R103"/>
+  <dimension ref="A1:R99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2520,6 +2520,9 @@
       <c r="C16" t="s">
         <v>289</v>
       </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
       <c r="E16" t="s">
         <v>439</v>
       </c>
@@ -2534,6 +2537,9 @@
       </c>
       <c r="O16" t="s">
         <v>234</v>
+      </c>
+      <c r="P16" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
@@ -2563,6 +2569,9 @@
       </c>
       <c r="O17" t="s">
         <v>235</v>
+      </c>
+      <c r="P17" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
@@ -3012,6 +3021,9 @@
       <c r="C31" t="s">
         <v>292</v>
       </c>
+      <c r="D31" s="2">
+        <v>1</v>
+      </c>
       <c r="E31" t="s">
         <v>399</v>
       </c>
@@ -3056,6 +3068,9 @@
       <c r="C32" t="s">
         <v>290</v>
       </c>
+      <c r="D32" s="2">
+        <v>1</v>
+      </c>
       <c r="E32" t="s">
         <v>398</v>
       </c>
@@ -3079,6 +3094,9 @@
       </c>
       <c r="M32" t="s">
         <v>135</v>
+      </c>
+      <c r="N32" s="2">
+        <v>1</v>
       </c>
       <c r="O32" t="s">
         <v>189</v>
@@ -3100,6 +3118,9 @@
       <c r="C33" t="s">
         <v>308</v>
       </c>
+      <c r="D33" s="2">
+        <v>0</v>
+      </c>
       <c r="E33" t="s">
         <v>430</v>
       </c>
@@ -3126,6 +3147,9 @@
       <c r="M33" t="s">
         <v>136</v>
       </c>
+      <c r="N33" s="2">
+        <v>1</v>
+      </c>
       <c r="O33" t="s">
         <v>95</v>
       </c>
@@ -3146,6 +3170,9 @@
       <c r="C34" t="s">
         <v>306</v>
       </c>
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
       <c r="E34" t="s">
         <v>431</v>
       </c>
@@ -3157,6 +3184,9 @@
       </c>
       <c r="M34" t="s">
         <v>138</v>
+      </c>
+      <c r="N34" s="2">
+        <v>1</v>
       </c>
       <c r="O34" t="s">
         <v>93</v>
@@ -3178,6 +3208,9 @@
       <c r="C35" t="s">
         <v>307</v>
       </c>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
       <c r="E35" t="s">
         <v>54</v>
       </c>
@@ -3194,6 +3227,9 @@
       <c r="M35" t="s">
         <v>137</v>
       </c>
+      <c r="N35" s="2">
+        <v>1</v>
+      </c>
       <c r="O35" t="s">
         <v>198</v>
       </c>
@@ -3226,6 +3262,9 @@
       <c r="M36" t="s">
         <v>142</v>
       </c>
+      <c r="N36" s="2">
+        <v>1</v>
+      </c>
       <c r="O36" t="s">
         <v>197</v>
       </c>
@@ -3258,6 +3297,9 @@
       <c r="M37" t="s">
         <v>140</v>
       </c>
+      <c r="N37" s="2">
+        <v>1</v>
+      </c>
       <c r="O37" t="s">
         <v>194</v>
       </c>
@@ -3291,6 +3333,9 @@
       <c r="M38" t="s">
         <v>139</v>
       </c>
+      <c r="N38" s="2">
+        <v>1</v>
+      </c>
       <c r="O38" t="s">
         <v>238</v>
       </c>
@@ -3317,6 +3362,9 @@
       <c r="M39" t="s">
         <v>141</v>
       </c>
+      <c r="N39" s="2">
+        <v>1</v>
+      </c>
       <c r="O39" t="s">
         <v>236</v>
       </c>
@@ -3345,7 +3393,7 @@
       </c>
       <c r="N40" s="2">
         <f>SUM(N32:N39)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O40" t="s">
         <v>207</v>
@@ -3453,6 +3501,9 @@
       <c r="C45" t="s">
         <v>301</v>
       </c>
+      <c r="D45" s="2">
+        <v>1</v>
+      </c>
       <c r="E45" t="s">
         <v>43</v>
       </c>
@@ -3461,6 +3512,9 @@
       </c>
       <c r="O45" t="s">
         <v>261</v>
+      </c>
+      <c r="P45" s="2">
+        <v>1</v>
       </c>
       <c r="Q45" t="s">
         <v>369</v>
@@ -3470,6 +3524,9 @@
       <c r="C46" t="s">
         <v>302</v>
       </c>
+      <c r="D46" s="2">
+        <v>1</v>
+      </c>
       <c r="E46" t="s">
         <v>396</v>
       </c>
@@ -3479,6 +3536,9 @@
       <c r="M46" s="1"/>
       <c r="O46" t="s">
         <v>260</v>
+      </c>
+      <c r="P46" s="2">
+        <v>1</v>
       </c>
       <c r="Q46" t="s">
         <v>149</v>
@@ -3489,6 +3549,9 @@
       <c r="B47" s="3"/>
       <c r="C47" t="s">
         <v>297</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1</v>
       </c>
       <c r="E47" t="s">
         <v>400</v>
@@ -3508,6 +3571,9 @@
       <c r="O47" t="s">
         <v>258</v>
       </c>
+      <c r="P47" s="2">
+        <v>1</v>
+      </c>
       <c r="Q47" t="s">
         <v>382</v>
       </c>
@@ -3516,6 +3582,9 @@
       <c r="C48" t="s">
         <v>298</v>
       </c>
+      <c r="D48" s="2">
+        <v>1</v>
+      </c>
       <c r="E48" t="s">
         <v>415</v>
       </c>
@@ -3551,6 +3620,9 @@
       <c r="C49" t="s">
         <v>299</v>
       </c>
+      <c r="D49" s="2">
+        <v>1</v>
+      </c>
       <c r="E49" t="s">
         <v>402</v>
       </c>
@@ -3595,6 +3667,9 @@
       <c r="C50" t="s">
         <v>300</v>
       </c>
+      <c r="D50" s="2">
+        <v>1</v>
+      </c>
       <c r="E50" t="s">
         <v>409</v>
       </c>
@@ -3628,6 +3703,9 @@
       </c>
       <c r="O50" t="s">
         <v>267</v>
+      </c>
+      <c r="P50" s="2">
+        <v>1</v>
       </c>
       <c r="Q50" t="s">
         <v>150</v>
@@ -3637,6 +3715,9 @@
       <c r="C51" t="s">
         <v>296</v>
       </c>
+      <c r="D51" s="2">
+        <v>1</v>
+      </c>
       <c r="E51" t="s">
         <v>51</v>
       </c>
@@ -3663,6 +3744,9 @@
       </c>
       <c r="O51" t="s">
         <v>265</v>
+      </c>
+      <c r="P51" s="2">
+        <v>1</v>
       </c>
       <c r="Q51" t="s">
         <v>381</v>
@@ -3674,7 +3758,7 @@
       </c>
       <c r="D52" s="2">
         <f>SUM(D2:D51)</f>
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E52" t="s">
         <v>419</v>
@@ -3853,11 +3937,11 @@
       </c>
       <c r="C57" s="12">
         <f>D52</f>
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D57" s="16">
         <f t="shared" ref="D57:D75" si="0">C57/B57</f>
-        <v>0.74</v>
+        <v>0.94</v>
       </c>
       <c r="E57" t="s">
         <v>394</v>
@@ -4068,6 +4152,9 @@
       <c r="O62" t="s">
         <v>262</v>
       </c>
+      <c r="P62" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A63" s="10" t="s">
@@ -4079,11 +4166,11 @@
       </c>
       <c r="C63" s="12">
         <f>P99</f>
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="D63" s="16">
         <f t="shared" si="0"/>
-        <v>0.88659793814432986</v>
+        <v>1</v>
       </c>
       <c r="E63" t="s">
         <v>49</v>
@@ -4099,6 +4186,9 @@
       </c>
       <c r="O63" t="s">
         <v>259</v>
+      </c>
+      <c r="P63" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4147,11 +4237,11 @@
       </c>
       <c r="C65" s="12">
         <f>F73</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D65" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>363</v>
@@ -4188,6 +4278,9 @@
       <c r="E66" t="s">
         <v>124</v>
       </c>
+      <c r="F66" s="2">
+        <v>1</v>
+      </c>
       <c r="I66" t="s">
         <v>335</v>
       </c>
@@ -4196,6 +4289,9 @@
       </c>
       <c r="O66" t="s">
         <v>268</v>
+      </c>
+      <c r="P66" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.35">
@@ -4217,6 +4313,9 @@
       <c r="E67" t="s">
         <v>126</v>
       </c>
+      <c r="F67" s="2">
+        <v>1</v>
+      </c>
       <c r="I67" t="s">
         <v>334</v>
       </c>
@@ -4225,6 +4324,9 @@
       </c>
       <c r="O67" t="s">
         <v>266</v>
+      </c>
+      <c r="P67" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.35">
@@ -4246,6 +4348,9 @@
       <c r="E68" t="s">
         <v>122</v>
       </c>
+      <c r="F68" s="2">
+        <v>1</v>
+      </c>
       <c r="I68" t="s">
         <v>336</v>
       </c>
@@ -4269,14 +4374,17 @@
       </c>
       <c r="C69" s="12">
         <f>N40</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D69" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E69" t="s">
         <v>121</v>
+      </c>
+      <c r="F69" s="2">
+        <v>1</v>
       </c>
       <c r="I69" t="s">
         <v>337</v>
@@ -4310,6 +4418,9 @@
       <c r="E70" t="s">
         <v>120</v>
       </c>
+      <c r="F70" s="2">
+        <v>1</v>
+      </c>
       <c r="I70" t="s">
         <v>344</v>
       </c>
@@ -4328,11 +4439,11 @@
         <v>387</v>
       </c>
       <c r="B71" s="9">
-        <f>E103</f>
+        <f>E95</f>
         <v>19</v>
       </c>
       <c r="C71" s="12">
-        <f>F103</f>
+        <f>F95</f>
         <v>19</v>
       </c>
       <c r="D71" s="16">
@@ -4341,6 +4452,9 @@
       </c>
       <c r="E71" t="s">
         <v>125</v>
+      </c>
+      <c r="F71" s="2">
+        <v>1</v>
       </c>
       <c r="I71" t="s">
         <v>443</v>
@@ -4374,6 +4488,9 @@
       <c r="E72" t="s">
         <v>123</v>
       </c>
+      <c r="F72" s="2">
+        <v>1</v>
+      </c>
       <c r="I72" t="s">
         <v>444</v>
       </c>
@@ -4408,7 +4525,7 @@
       </c>
       <c r="F73" s="2">
         <f>SUM(F66:F72)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I73" t="s">
         <v>340</v>
@@ -4423,7 +4540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="10" t="s">
         <v>317</v>
       </c>
@@ -4467,6 +4584,9 @@
       <c r="D75" s="16">
         <f t="shared" si="0"/>
         <v>1</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>387</v>
       </c>
       <c r="I75" t="s">
         <v>342</v>
@@ -4486,6 +4606,12 @@
       <c r="B76" s="9"/>
       <c r="C76" s="12"/>
       <c r="D76" s="9"/>
+      <c r="E76" t="s">
+        <v>183</v>
+      </c>
+      <c r="F76" s="2">
+        <v>1</v>
+      </c>
       <c r="I76" t="s">
         <v>343</v>
       </c>
@@ -4507,9 +4633,15 @@
       </c>
       <c r="C77" s="12">
         <f>SUM(C56:C76)</f>
-        <v>339</v>
+        <v>375</v>
       </c>
       <c r="D77" s="9"/>
+      <c r="E77" t="s">
+        <v>184</v>
+      </c>
+      <c r="F77" s="2">
+        <v>1</v>
+      </c>
       <c r="I77" t="s">
         <v>353</v>
       </c>
@@ -4527,10 +4659,16 @@
       <c r="A78" s="13"/>
       <c r="B78" s="14">
         <f>C77/B77</f>
-        <v>0.79952830188679247</v>
+        <v>0.88443396226415094</v>
       </c>
       <c r="C78" s="13"/>
       <c r="D78" s="9"/>
+      <c r="E78" t="s">
+        <v>180</v>
+      </c>
+      <c r="F78" s="2">
+        <v>1</v>
+      </c>
       <c r="I78" t="s">
         <v>347</v>
       </c>
@@ -4545,6 +4683,12 @@
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E79" t="s">
+        <v>181</v>
+      </c>
+      <c r="F79" s="2">
+        <v>1</v>
+      </c>
       <c r="I79" t="s">
         <v>348</v>
       </c>
@@ -4559,6 +4703,12 @@
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E80" t="s">
+        <v>182</v>
+      </c>
+      <c r="F80" s="2">
+        <v>1</v>
+      </c>
       <c r="I80" t="s">
         <v>349</v>
       </c>
@@ -4573,6 +4723,12 @@
       </c>
     </row>
     <row r="81" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E81" t="s">
+        <v>176</v>
+      </c>
+      <c r="F81" s="2">
+        <v>1</v>
+      </c>
       <c r="I81" t="s">
         <v>445</v>
       </c>
@@ -4586,9 +4742,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="5:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E82" s="1"/>
-      <c r="F82" s="3"/>
+    <row r="82" spans="5:16" x14ac:dyDescent="0.35">
+      <c r="E82" t="s">
+        <v>174</v>
+      </c>
+      <c r="F82" s="2">
+        <v>1</v>
+      </c>
       <c r="I82" t="s">
         <v>361</v>
       </c>
@@ -4603,8 +4763,11 @@
       </c>
     </row>
     <row r="83" spans="5:16" x14ac:dyDescent="0.35">
-      <c r="E83" s="6" t="s">
-        <v>387</v>
+      <c r="E83" t="s">
+        <v>173</v>
+      </c>
+      <c r="F83" s="2">
+        <v>1</v>
       </c>
       <c r="I83" t="s">
         <v>352</v>
@@ -4621,7 +4784,7 @@
     </row>
     <row r="84" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E84" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="F84" s="2">
         <v>1</v>
@@ -4641,7 +4804,7 @@
     </row>
     <row r="85" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E85" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="F85" s="2">
         <v>1</v>
@@ -4661,7 +4824,7 @@
     </row>
     <row r="86" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E86" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="F86" s="2">
         <v>1</v>
@@ -4681,7 +4844,7 @@
     </row>
     <row r="87" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E87" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="F87" s="2">
         <v>1</v>
@@ -4701,7 +4864,7 @@
     </row>
     <row r="88" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E88" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="F88" s="2">
         <v>1</v>
@@ -4721,7 +4884,7 @@
     </row>
     <row r="89" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E89" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="F89" s="2">
         <v>1</v>
@@ -4741,7 +4904,7 @@
     </row>
     <row r="90" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E90" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="F90" s="2">
         <v>1</v>
@@ -4762,7 +4925,7 @@
     </row>
     <row r="91" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E91" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F91" s="2">
         <v>1</v>
@@ -4776,7 +4939,7 @@
     </row>
     <row r="92" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E92" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="F92" s="2">
         <v>1</v>
@@ -4790,7 +4953,7 @@
     </row>
     <row r="93" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E93" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="F93" s="2">
         <v>1</v>
@@ -4804,7 +4967,7 @@
     </row>
     <row r="94" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E94" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="F94" s="2">
         <v>1</v>
@@ -4817,11 +4980,12 @@
       </c>
     </row>
     <row r="95" spans="5:16" x14ac:dyDescent="0.35">
-      <c r="E95" t="s">
-        <v>171</v>
+      <c r="E95" s="4">
+        <v>19</v>
       </c>
       <c r="F95" s="2">
-        <v>1</v>
+        <f>SUM(F76:F94)</f>
+        <v>19</v>
       </c>
       <c r="O95" t="s">
         <v>219</v>
@@ -4831,12 +4995,6 @@
       </c>
     </row>
     <row r="96" spans="5:16" x14ac:dyDescent="0.35">
-      <c r="E96" t="s">
-        <v>169</v>
-      </c>
-      <c r="F96" s="2">
-        <v>1</v>
-      </c>
       <c r="O96" t="s">
         <v>218</v>
       </c>
@@ -4844,13 +5002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="5:16" x14ac:dyDescent="0.35">
-      <c r="E97" t="s">
-        <v>168</v>
-      </c>
-      <c r="F97" s="2">
-        <v>1</v>
-      </c>
+    <row r="97" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O97" t="s">
         <v>217</v>
       </c>
@@ -4858,13 +5010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="5:16" x14ac:dyDescent="0.35">
-      <c r="E98" t="s">
-        <v>167</v>
-      </c>
-      <c r="F98" s="2">
-        <v>1</v>
-      </c>
+    <row r="98" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O98" t="s">
         <v>216</v>
       </c>
@@ -4872,52 +5018,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="5:16" x14ac:dyDescent="0.35">
-      <c r="E99" t="s">
-        <v>170</v>
-      </c>
-      <c r="F99" s="2">
-        <v>1</v>
-      </c>
+    <row r="99" spans="15:16" x14ac:dyDescent="0.35">
       <c r="O99" s="4">
         <v>97</v>
       </c>
       <c r="P99" s="2">
         <f>SUM(P2:P98)</f>
-        <v>86</v>
-      </c>
-    </row>
-    <row r="100" spans="5:16" x14ac:dyDescent="0.35">
-      <c r="E100" t="s">
-        <v>177</v>
-      </c>
-      <c r="F100" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="5:16" x14ac:dyDescent="0.35">
-      <c r="E101" t="s">
-        <v>179</v>
-      </c>
-      <c r="F101" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="5:16" x14ac:dyDescent="0.35">
-      <c r="E102" t="s">
-        <v>178</v>
-      </c>
-      <c r="F102" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="5:16" x14ac:dyDescent="0.35">
-      <c r="E103" s="4">
-        <v>19</v>
-      </c>
-      <c r="F103" s="2">
-        <f>SUM(F84:F102)</f>
-        <v>19</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Progressive rendering, Struct Trees & Struct Elements (backed by TaggedObject).
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\coding\dotPDFium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C24D8C2-83B2-44BC-A6FC-FB5E646C1EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194E5186-2EC7-4A4A-A06E-B6C56FA42C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="930" windowWidth="36190" windowHeight="19510" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
+    <workbookView xWindow="40400" yWindow="710" windowWidth="36190" windowHeight="19510" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="448">
   <si>
     <t>Text_LoadPage</t>
   </si>
@@ -1374,6 +1374,12 @@
   </si>
   <si>
     <t>FORM_SetFocusedAnnot</t>
+  </si>
+  <si>
+    <t>StructElement_GetAttr</t>
+  </si>
+  <si>
+    <t>StructElement_GetMarkedContentIdCount</t>
   </si>
 </sst>
 </file>
@@ -1500,10 +1506,10 @@
     <xf numFmtId="10" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1843,7 +1849,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93991F7-7A9D-4291-8EC0-AB472EBDEDBD}">
   <dimension ref="A1:R99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1924,6 +1932,9 @@
       <c r="I2" t="s">
         <v>66</v>
       </c>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
       <c r="K2" t="s">
         <v>68</v>
       </c>
@@ -1974,6 +1985,9 @@
       <c r="I3" t="s">
         <v>67</v>
       </c>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
       <c r="K3" t="s">
         <v>69</v>
       </c>
@@ -2026,7 +2040,7 @@
       </c>
       <c r="J4" s="2">
         <f>SUM(J2:J3)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K4" t="s">
         <v>71</v>
@@ -3033,6 +3047,9 @@
       <c r="G31" t="s">
         <v>130</v>
       </c>
+      <c r="H31" s="2">
+        <v>1</v>
+      </c>
       <c r="I31" t="s">
         <v>131</v>
       </c>
@@ -3056,6 +3073,9 @@
       </c>
       <c r="Q31" s="7" t="s">
         <v>379</v>
+      </c>
+      <c r="R31" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.35">
@@ -3080,6 +3100,9 @@
       <c r="G32" t="s">
         <v>129</v>
       </c>
+      <c r="H32" s="2">
+        <v>1</v>
+      </c>
       <c r="I32" t="s">
         <v>132</v>
       </c>
@@ -3107,8 +3130,11 @@
       <c r="Q32" s="7" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -3129,6 +3155,9 @@
       </c>
       <c r="G33" t="s">
         <v>127</v>
+      </c>
+      <c r="H33" s="2">
+        <v>1</v>
       </c>
       <c r="I33" s="4">
         <v>2</v>
@@ -3159,8 +3188,11 @@
       <c r="Q33" s="7" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>272</v>
       </c>
@@ -3182,6 +3214,9 @@
       <c r="G34" t="s">
         <v>128</v>
       </c>
+      <c r="H34" s="2">
+        <v>1</v>
+      </c>
       <c r="M34" t="s">
         <v>138</v>
       </c>
@@ -3197,8 +3232,11 @@
       <c r="Q34" s="7" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R34" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>270</v>
       </c>
@@ -3222,7 +3260,7 @@
       </c>
       <c r="H35" s="2">
         <f>SUM(H31:H34)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M35" t="s">
         <v>137</v>
@@ -3239,8 +3277,11 @@
       <c r="Q35" s="7" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R35" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>271</v>
       </c>
@@ -3274,8 +3315,11 @@
       <c r="Q36" s="7" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -3309,8 +3353,11 @@
       <c r="Q37" s="7" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R37" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -3345,8 +3392,11 @@
       <c r="Q38" s="7" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R38" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C39" t="s">
         <v>19</v>
       </c>
@@ -3374,8 +3424,11 @@
       <c r="Q39" s="7" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R39" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C40" t="s">
         <v>20</v>
       </c>
@@ -3404,8 +3457,11 @@
       <c r="Q40" s="7" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R40" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C41" t="s">
         <v>23</v>
       </c>
@@ -3427,8 +3483,11 @@
       <c r="Q41" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R41" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C42" t="s">
         <v>41</v>
       </c>
@@ -3450,8 +3509,11 @@
       <c r="Q42" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R42" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C43" t="s">
         <v>38</v>
       </c>
@@ -3473,8 +3535,11 @@
       <c r="Q43" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R43" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C44" t="s">
         <v>39</v>
       </c>
@@ -3494,10 +3559,13 @@
         <v>1</v>
       </c>
       <c r="Q44" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+        <v>446</v>
+      </c>
+      <c r="R44" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C45" t="s">
         <v>301</v>
       </c>
@@ -3517,10 +3585,13 @@
         <v>1</v>
       </c>
       <c r="Q45" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>370</v>
+      </c>
+      <c r="R45" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C46" t="s">
         <v>302</v>
       </c>
@@ -3541,10 +3612,13 @@
         <v>1</v>
       </c>
       <c r="Q46" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>369</v>
+      </c>
+      <c r="R46" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="1"/>
       <c r="B47" s="3"/>
       <c r="C47" t="s">
@@ -3575,10 +3649,13 @@
         <v>1</v>
       </c>
       <c r="Q47" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+      <c r="R47" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C48" t="s">
         <v>298</v>
       </c>
@@ -3613,7 +3690,10 @@
         <v>1</v>
       </c>
       <c r="Q48" t="s">
-        <v>153</v>
+        <v>382</v>
+      </c>
+      <c r="R48" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.35">
@@ -3660,7 +3740,10 @@
         <v>1</v>
       </c>
       <c r="Q49" t="s">
-        <v>154</v>
+        <v>153</v>
+      </c>
+      <c r="R49" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.35">
@@ -3708,7 +3791,10 @@
         <v>1</v>
       </c>
       <c r="Q50" t="s">
-        <v>150</v>
+        <v>154</v>
+      </c>
+      <c r="R50" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.35">
@@ -3749,7 +3835,10 @@
         <v>1</v>
       </c>
       <c r="Q51" t="s">
-        <v>381</v>
+        <v>150</v>
+      </c>
+      <c r="R51" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.35">
@@ -3792,7 +3881,10 @@
         <v>1</v>
       </c>
       <c r="Q52" t="s">
-        <v>156</v>
+        <v>447</v>
+      </c>
+      <c r="R52" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.35">
@@ -3821,7 +3913,10 @@
         <v>1</v>
       </c>
       <c r="Q53" t="s">
-        <v>148</v>
+        <v>381</v>
+      </c>
+      <c r="R53" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.35">
@@ -3850,15 +3945,18 @@
         <v>1</v>
       </c>
       <c r="Q54" t="s">
-        <v>383</v>
+        <v>156</v>
+      </c>
+      <c r="R54" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A55" s="15" t="s">
+      <c r="A55" s="16" t="s">
         <v>388</v>
       </c>
-      <c r="B55" s="15"/>
-      <c r="C55" s="15"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="16"/>
       <c r="D55" s="11"/>
       <c r="E55" t="s">
         <v>442</v>
@@ -3886,7 +3984,10 @@
         <v>1</v>
       </c>
       <c r="Q55" t="s">
-        <v>157</v>
+        <v>148</v>
+      </c>
+      <c r="R55" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.35">
@@ -3901,7 +4002,7 @@
         <f>B38</f>
         <v>36</v>
       </c>
-      <c r="D56" s="16">
+      <c r="D56" s="15">
         <f>C56/B56</f>
         <v>1</v>
       </c>
@@ -3924,7 +4025,10 @@
         <v>1</v>
       </c>
       <c r="Q56" t="s">
-        <v>155</v>
+        <v>383</v>
+      </c>
+      <c r="R56" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.35">
@@ -3939,7 +4043,7 @@
         <f>D52</f>
         <v>47</v>
       </c>
-      <c r="D57" s="16">
+      <c r="D57" s="15">
         <f t="shared" ref="D57:D75" si="0">C57/B57</f>
         <v>0.94</v>
       </c>
@@ -3962,7 +4066,10 @@
         <v>1</v>
       </c>
       <c r="Q57" t="s">
-        <v>144</v>
+        <v>157</v>
+      </c>
+      <c r="R57" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.35">
@@ -3977,7 +4084,7 @@
         <f>F64</f>
         <v>61</v>
       </c>
-      <c r="D58" s="16">
+      <c r="D58" s="15">
         <f t="shared" si="0"/>
         <v>0.9838709677419355</v>
       </c>
@@ -4000,7 +4107,10 @@
         <v>1</v>
       </c>
       <c r="Q58" t="s">
-        <v>145</v>
+        <v>155</v>
+      </c>
+      <c r="R58" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.35">
@@ -4015,7 +4125,7 @@
         <f>H14</f>
         <v>12</v>
       </c>
-      <c r="D59" s="16">
+      <c r="D59" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4038,7 +4148,10 @@
         <v>1</v>
       </c>
       <c r="Q59" t="s">
-        <v>146</v>
+        <v>144</v>
+      </c>
+      <c r="R59" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.35">
@@ -4051,11 +4164,11 @@
       </c>
       <c r="C60" s="12">
         <f>J4</f>
-        <v>0</v>
-      </c>
-      <c r="D60" s="16">
+        <v>2</v>
+      </c>
+      <c r="D60" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60" t="s">
         <v>46</v>
@@ -4076,10 +4189,13 @@
         <v>1</v>
       </c>
       <c r="Q60" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>145</v>
+      </c>
+      <c r="R60" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A61" s="10" t="s">
         <v>315</v>
       </c>
@@ -4091,7 +4207,7 @@
         <f>L10</f>
         <v>0</v>
       </c>
-      <c r="D61" s="16">
+      <c r="D61" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4113,12 +4229,11 @@
       <c r="P61" s="2">
         <v>1</v>
       </c>
-      <c r="Q61" s="8">
-        <v>29</v>
-      </c>
-      <c r="R61" s="3">
-        <f>SUM(R31:R60)</f>
-        <v>0</v>
+      <c r="Q61" t="s">
+        <v>146</v>
+      </c>
+      <c r="R61" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.35">
@@ -4133,7 +4248,7 @@
         <f>N30</f>
         <v>27</v>
       </c>
-      <c r="D62" s="16">
+      <c r="D62" s="15">
         <f t="shared" si="0"/>
         <v>0.9642857142857143</v>
       </c>
@@ -4155,8 +4270,14 @@
       <c r="P62" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="Q62" t="s">
+        <v>143</v>
+      </c>
+      <c r="R62" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="10" t="s">
         <v>389</v>
       </c>
@@ -4168,7 +4289,7 @@
         <f>P99</f>
         <v>97</v>
       </c>
-      <c r="D63" s="16">
+      <c r="D63" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4189,6 +4310,13 @@
       </c>
       <c r="P63" s="2">
         <v>1</v>
+      </c>
+      <c r="Q63" s="8">
+        <v>32</v>
+      </c>
+      <c r="R63" s="3">
+        <f>SUM(R31:R62)</f>
+        <v>32</v>
       </c>
     </row>
     <row r="64" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4203,7 +4331,7 @@
         <f>R8</f>
         <v>6</v>
       </c>
-      <c r="D64" s="16">
+      <c r="D64" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4239,7 +4367,7 @@
         <f>F73</f>
         <v>7</v>
       </c>
-      <c r="D65" s="16">
+      <c r="D65" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4269,11 +4397,11 @@
       </c>
       <c r="C66" s="12">
         <f>H35</f>
-        <v>0</v>
-      </c>
-      <c r="D66" s="16">
+        <v>4</v>
+      </c>
+      <c r="D66" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E66" t="s">
         <v>124</v>
@@ -4306,7 +4434,7 @@
         <f>J33</f>
         <v>2</v>
       </c>
-      <c r="D67" s="16">
+      <c r="D67" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4341,7 +4469,7 @@
         <f>L33</f>
         <v>2</v>
       </c>
-      <c r="D68" s="16">
+      <c r="D68" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4376,7 +4504,7 @@
         <f>N40</f>
         <v>8</v>
       </c>
-      <c r="D69" s="16">
+      <c r="D69" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4404,16 +4532,16 @@
         <v>368</v>
       </c>
       <c r="B70" s="9">
-        <f>Q61</f>
-        <v>29</v>
+        <f>Q63</f>
+        <v>32</v>
       </c>
       <c r="C70" s="12">
-        <f>R61</f>
-        <v>0</v>
-      </c>
-      <c r="D70" s="16">
+        <f>R63</f>
+        <v>32</v>
+      </c>
+      <c r="D70" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E70" t="s">
         <v>120</v>
@@ -4446,7 +4574,7 @@
         <f>F95</f>
         <v>19</v>
       </c>
-      <c r="D71" s="16">
+      <c r="D71" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4481,7 +4609,7 @@
         <f>H52</f>
         <v>3</v>
       </c>
-      <c r="D72" s="16">
+      <c r="D72" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4516,7 +4644,7 @@
         <f>J90</f>
         <v>40</v>
       </c>
-      <c r="D73" s="16">
+      <c r="D73" s="15">
         <f t="shared" si="0"/>
         <v>0.97560975609756095</v>
       </c>
@@ -4552,7 +4680,7 @@
         <f>L50</f>
         <v>1</v>
       </c>
-      <c r="D74" s="16">
+      <c r="D74" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4581,7 +4709,7 @@
         <f>N55</f>
         <v>7</v>
       </c>
-      <c r="D75" s="16">
+      <c r="D75" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4629,11 +4757,11 @@
       <c r="A77" s="10"/>
       <c r="B77" s="9">
         <f>SUM(B56:B76)</f>
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="C77" s="12">
         <f>SUM(C56:C76)</f>
-        <v>375</v>
+        <v>413</v>
       </c>
       <c r="D77" s="9"/>
       <c r="E77" t="s">
@@ -4659,7 +4787,7 @@
       <c r="A78" s="13"/>
       <c r="B78" s="14">
         <f>C77/B77</f>
-        <v>0.88443396226415094</v>
+        <v>0.96721311475409832</v>
       </c>
       <c r="C78" s="13"/>
       <c r="D78" s="9"/>

</xml_diff>

<commit_message>
Implemented availability / document streaming support.
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\coding\dotPDFium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194E5186-2EC7-4A4A-A06E-B6C56FA42C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23495265-379C-4153-9AAD-5CE3E0E843CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40400" yWindow="710" windowWidth="36190" windowHeight="19510" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
+    <workbookView xWindow="4060" yWindow="1740" windowWidth="30310" windowHeight="15080" xr2:uid="{86B723CF-4BB8-4652-A711-183346CF315A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1849,8 +1849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93991F7-7A9D-4291-8EC0-AB472EBDEDBD}">
   <dimension ref="A1:R99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1938,6 +1938,9 @@
       <c r="K2" t="s">
         <v>68</v>
       </c>
+      <c r="L2" s="2">
+        <v>1</v>
+      </c>
       <c r="M2" t="s">
         <v>84</v>
       </c>
@@ -1991,6 +1994,9 @@
       <c r="K3" t="s">
         <v>69</v>
       </c>
+      <c r="L3" s="2">
+        <v>1</v>
+      </c>
       <c r="M3" t="s">
         <v>85</v>
       </c>
@@ -2045,6 +2051,9 @@
       <c r="K4" t="s">
         <v>71</v>
       </c>
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
       <c r="M4" t="s">
         <v>83</v>
       </c>
@@ -2092,6 +2101,9 @@
       <c r="K5" t="s">
         <v>75</v>
       </c>
+      <c r="L5" s="2">
+        <v>1</v>
+      </c>
       <c r="M5" t="s">
         <v>86</v>
       </c>
@@ -2139,6 +2151,9 @@
       <c r="K6" t="s">
         <v>70</v>
       </c>
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
       <c r="M6" t="s">
         <v>82</v>
       </c>
@@ -2186,6 +2201,9 @@
       <c r="K7" t="s">
         <v>73</v>
       </c>
+      <c r="L7" s="2">
+        <v>1</v>
+      </c>
       <c r="M7" t="s">
         <v>80</v>
       </c>
@@ -2233,6 +2251,9 @@
       <c r="K8" t="s">
         <v>74</v>
       </c>
+      <c r="L8" s="2">
+        <v>1</v>
+      </c>
       <c r="M8" t="s">
         <v>81</v>
       </c>
@@ -2281,6 +2302,9 @@
       <c r="K9" t="s">
         <v>72</v>
       </c>
+      <c r="L9" s="2">
+        <v>1</v>
+      </c>
       <c r="M9" t="s">
         <v>79</v>
       </c>
@@ -2324,7 +2348,7 @@
       </c>
       <c r="L10" s="2">
         <f>SUM(L2:L9)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M10" t="s">
         <v>76</v>
@@ -2803,7 +2827,7 @@
         <v>319</v>
       </c>
       <c r="N24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O24" t="s">
         <v>253</v>
@@ -3013,7 +3037,7 @@
       </c>
       <c r="N30" s="3">
         <f>SUM(N2:N29)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O30" t="s">
         <v>98</v>
@@ -4205,11 +4229,11 @@
       </c>
       <c r="C61" s="12">
         <f>L10</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D61" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E61" t="s">
         <v>45</v>
@@ -4246,11 +4270,11 @@
       </c>
       <c r="C62" s="12">
         <f>N30</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D62" s="15">
         <f t="shared" si="0"/>
-        <v>0.9642857142857143</v>
+        <v>1</v>
       </c>
       <c r="E62" t="s">
         <v>47</v>
@@ -4761,7 +4785,7 @@
       </c>
       <c r="C77" s="12">
         <f>SUM(C56:C76)</f>
-        <v>413</v>
+        <v>422</v>
       </c>
       <c r="D77" s="9"/>
       <c r="E77" t="s">
@@ -4787,7 +4811,7 @@
       <c r="A78" s="13"/>
       <c r="B78" s="14">
         <f>C77/B77</f>
-        <v>0.96721311475409832</v>
+        <v>0.98829039812646369</v>
       </c>
       <c r="C78" s="13"/>
       <c r="D78" s="9"/>

</xml_diff>